<commit_message>
Matrice des corrélations systématiques
</commit_message>
<xml_diff>
--- a/scripts/Edouard/Correlation_matrix.xlsx
+++ b/scripts/Edouard/Correlation_matrix.xlsx
@@ -19,15 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> Outliers : TRUE ; Outliers_coef : 10 ; Trans_number : 0 ; Prod_problems : TRUE ; Product_select : FALSE ; Remove_double : TRUE ; Ponderation : TRUE ; Pond_log : FALSE ;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Outliers : TRUE ; Outliers_coef : 3.5 ; Trans_number : 0 ; Prod_problems : TRUE ; Product_select : FALSE ; Remove_double : TRUE ; Ponderation : TRUE ; Pond_log : FALSE ;</t>
   </si>
   <si>
     <t xml:space="preserve"> Outliers : FALSE ; Outliers_coef : 3.5 ; Trans_number : 0 ; Prod_problems : FALSE ; Product_select : FALSE ; Remove_double : TRUE ; Ponderation : TRUE ; Pond_log : FALSE ;</t>
@@ -46,6 +40,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Outliers : TRUE ; Outliers_coef : 3.5 ; Trans_number : 0 ; Prod_problems : FALSE ; Product_select : FALSE ; Remove_double : FALSE ; Ponderation : TRUE ; Pond_log : FALSE ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Outliers : TRUE ; Outliers_coef : 3.5 ; Trans_number : 0 ; Prod_problems : FALSE ; Product_select : FALSE ; Remove_double : TRUE ; Ponderation : FALSE ; Pond_log : FALSE ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Outliers : TRUE ; Outliers_coef : 3.5 ; Trans_number : 0 ; Prod_problems : FALSE ; Product_select : FALSE ; Remove_double : TRUE ; Ponderation : TRUE ; Pond_log : TRUE ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Outliers : TRUE ; Outliers_coef : 3.5 ; Trans_number : 0 ; Prod_problems : TRUE ; Product_select : FALSE ; Remove_double : TRUE ; Ponderation : TRUE ; Pond_log : FALSE ;</t>
   </si>
 </sst>
 </file>
@@ -405,6 +408,9 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -414,25 +420,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.653342754964692</v>
+        <v>0.901804218632853</v>
       </c>
       <c r="D2" t="n">
-        <v>0.909504651891034</v>
+        <v>0.356194649740909</v>
       </c>
       <c r="E2" t="n">
-        <v>0.998177204562645</v>
+        <v>0.435519780609543</v>
       </c>
       <c r="F2" t="n">
-        <v>0.484202971159519</v>
+        <v>0.458418296887294</v>
       </c>
       <c r="G2" t="n">
-        <v>0.623127722947945</v>
+        <v>0.733437290156057</v>
       </c>
       <c r="H2" t="n">
-        <v>0.588634783690962</v>
+        <v>0.806699412156276</v>
       </c>
       <c r="I2" t="n">
-        <v>0.880083858871079</v>
+        <v>0.829515381238252</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.462976500925549</v>
       </c>
     </row>
     <row r="3">
@@ -440,28 +449,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.653342754964692</v>
+        <v>0.901804218632853</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.462976500925549</v>
+        <v>0.509983922154108</v>
       </c>
       <c r="E3" t="n">
+        <v>0.648756494372831</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.606206977827473</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.889843101802611</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.681576636415055</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.726771597449783</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.674230460908826</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.935855024521929</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.99612934757487</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.925827314057919</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.78801119700484</v>
       </c>
     </row>
     <row r="4">
@@ -469,28 +481,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.909504651891034</v>
+        <v>0.356194649740909</v>
       </c>
       <c r="C4" t="n">
-        <v>0.462976500925549</v>
+        <v>0.509983922154108</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.901804218632853</v>
+        <v>0.945919536392486</v>
       </c>
       <c r="F4" t="n">
-        <v>0.356194649740909</v>
+        <v>0.925148662955917</v>
       </c>
       <c r="G4" t="n">
-        <v>0.435519780609543</v>
+        <v>0.626115640850283</v>
       </c>
       <c r="H4" t="n">
-        <v>0.458418296887294</v>
+        <v>0.13812017166833</v>
       </c>
       <c r="I4" t="n">
-        <v>0.733437290156057</v>
+        <v>0.155712844922479</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.935855024521929</v>
       </c>
     </row>
     <row r="5">
@@ -498,28 +513,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.998177204562645</v>
+        <v>0.435519780609543</v>
       </c>
       <c r="C5" t="n">
-        <v>0.674230460908826</v>
+        <v>0.648756494372831</v>
       </c>
       <c r="D5" t="n">
-        <v>0.901804218632853</v>
+        <v>0.945919536392486</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.509983922154108</v>
+        <v>0.921162587247194</v>
       </c>
       <c r="G5" t="n">
-        <v>0.648756494372831</v>
+        <v>0.7706107038364</v>
       </c>
       <c r="H5" t="n">
-        <v>0.606206977827473</v>
+        <v>0.196686159916996</v>
       </c>
       <c r="I5" t="n">
-        <v>0.889843101802611</v>
+        <v>0.237231030273605</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.99612934757487</v>
       </c>
     </row>
     <row r="6">
@@ -527,28 +545,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.484202971159519</v>
+        <v>0.458418296887294</v>
       </c>
       <c r="C6" t="n">
-        <v>0.935855024521929</v>
+        <v>0.606206977827473</v>
       </c>
       <c r="D6" t="n">
-        <v>0.356194649740909</v>
+        <v>0.925148662955917</v>
       </c>
       <c r="E6" t="n">
-        <v>0.509983922154108</v>
+        <v>0.921162587247194</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.945919536392486</v>
+        <v>0.762835256792117</v>
       </c>
       <c r="H6" t="n">
-        <v>0.925148662955917</v>
+        <v>0.219368230834023</v>
       </c>
       <c r="I6" t="n">
-        <v>0.626115640850283</v>
+        <v>0.225653261515404</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.925827314057919</v>
       </c>
     </row>
     <row r="7">
@@ -556,28 +577,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.623127722947945</v>
+        <v>0.733437290156057</v>
       </c>
       <c r="C7" t="n">
-        <v>0.99612934757487</v>
+        <v>0.889843101802611</v>
       </c>
       <c r="D7" t="n">
-        <v>0.435519780609543</v>
+        <v>0.626115640850283</v>
       </c>
       <c r="E7" t="n">
-        <v>0.648756494372831</v>
+        <v>0.7706107038364</v>
       </c>
       <c r="F7" t="n">
-        <v>0.945919536392486</v>
+        <v>0.762835256792117</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.921162587247194</v>
+        <v>0.490274942033487</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7706107038364</v>
+        <v>0.531082419831071</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.78801119700484</v>
       </c>
     </row>
     <row r="8">
@@ -585,28 +609,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.588634783690962</v>
+        <v>0.806699412156276</v>
       </c>
       <c r="C8" t="n">
-        <v>0.925827314057919</v>
+        <v>0.681576636415055</v>
       </c>
       <c r="D8" t="n">
-        <v>0.458418296887294</v>
+        <v>0.13812017166833</v>
       </c>
       <c r="E8" t="n">
-        <v>0.606206977827473</v>
+        <v>0.196686159916996</v>
       </c>
       <c r="F8" t="n">
-        <v>0.925148662955917</v>
+        <v>0.219368230834023</v>
       </c>
       <c r="G8" t="n">
-        <v>0.921162587247194</v>
+        <v>0.490274942033487</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.762835256792117</v>
+        <v>0.990347129933348</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.217741007283888</v>
       </c>
     </row>
     <row r="9">
@@ -614,27 +641,62 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.880083858871079</v>
+        <v>0.829515381238252</v>
       </c>
       <c r="C9" t="n">
+        <v>0.726771597449783</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.155712844922479</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.237231030273605</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.225653261515404</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.531082419831071</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.990347129933348</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.257989742803437</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.462976500925549</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.674230460908826</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.935855024521929</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.99612934757487</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.925827314057919</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.78801119700484</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.733437290156057</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.889843101802611</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.626115640850283</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.7706107038364</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.762835256792117</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="H10" t="n">
+        <v>0.217741007283888</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.257989742803437</v>
+      </c>
+      <c r="J10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -680,6 +742,9 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -689,25 +754,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.834389070974318</v>
+        <v>0.22339520763975</v>
       </c>
       <c r="D2" t="n">
-        <v>0.221918391528785</v>
+        <v>0.77372598741087</v>
       </c>
       <c r="E2" t="n">
-        <v>0.999768750645947</v>
+        <v>0.638697250451824</v>
       </c>
       <c r="F2" t="n">
-        <v>0.683402758279144</v>
+        <v>0.44716708401268</v>
       </c>
       <c r="G2" t="n">
-        <v>0.833683034767251</v>
+        <v>0.476329863035688</v>
       </c>
       <c r="H2" t="n">
-        <v>0.724759269901657</v>
+        <v>0.438820638841603</v>
       </c>
       <c r="I2" t="n">
-        <v>0.764551818279103</v>
+        <v>0.424123380735669</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.638096956923035</v>
       </c>
     </row>
     <row r="3">
@@ -715,28 +783,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.834389070974318</v>
+        <v>0.22339520763975</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.638096956923035</v>
+        <v>0.684885362084019</v>
       </c>
       <c r="E3" t="n">
+        <v>0.835006156623799</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.729186065614364</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.763140667579433</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.722969574589664</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.733119324885382</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.835647840454511</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.945880995727681</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.999977186256954</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.825306777206141</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.866428171542027</v>
       </c>
     </row>
     <row r="4">
@@ -744,28 +815,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.221918391528785</v>
+        <v>0.77372598741087</v>
       </c>
       <c r="C4" t="n">
-        <v>0.638096956923035</v>
+        <v>0.684885362084019</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.22339520763975</v>
+        <v>0.946115214989885</v>
       </c>
       <c r="F4" t="n">
-        <v>0.77372598741087</v>
+        <v>0.727100492243932</v>
       </c>
       <c r="G4" t="n">
-        <v>0.638697250451824</v>
+        <v>0.780784036855754</v>
       </c>
       <c r="H4" t="n">
-        <v>0.44716708401268</v>
+        <v>0.708063599850068</v>
       </c>
       <c r="I4" t="n">
-        <v>0.476329863035688</v>
+        <v>0.692229881668236</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.945880995727681</v>
       </c>
     </row>
     <row r="5">
@@ -773,28 +847,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.999768750645947</v>
+        <v>0.638697250451824</v>
       </c>
       <c r="C5" t="n">
-        <v>0.835647840454511</v>
+        <v>0.835006156623799</v>
       </c>
       <c r="D5" t="n">
-        <v>0.22339520763975</v>
+        <v>0.946115214989885</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.684885362084019</v>
+        <v>0.826369426010633</v>
       </c>
       <c r="G5" t="n">
-        <v>0.835006156623799</v>
+        <v>0.866088097442708</v>
       </c>
       <c r="H5" t="n">
-        <v>0.729186065614364</v>
+        <v>0.767516242826121</v>
       </c>
       <c r="I5" t="n">
-        <v>0.763140667579433</v>
+        <v>0.769218318413894</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.999977186256954</v>
       </c>
     </row>
     <row r="6">
@@ -802,28 +879,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.683402758279144</v>
+        <v>0.44716708401268</v>
       </c>
       <c r="C6" t="n">
-        <v>0.945880995727681</v>
+        <v>0.729186065614364</v>
       </c>
       <c r="D6" t="n">
-        <v>0.77372598741087</v>
+        <v>0.727100492243932</v>
       </c>
       <c r="E6" t="n">
-        <v>0.684885362084019</v>
+        <v>0.826369426010633</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.946115214989885</v>
+        <v>0.693971325525491</v>
       </c>
       <c r="H6" t="n">
-        <v>0.727100492243932</v>
+        <v>0.686000509241168</v>
       </c>
       <c r="I6" t="n">
-        <v>0.780784036855754</v>
+        <v>0.71172756770144</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.825306777206141</v>
       </c>
     </row>
     <row r="7">
@@ -831,28 +911,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.833683034767251</v>
+        <v>0.476329863035688</v>
       </c>
       <c r="C7" t="n">
-        <v>0.999977186256954</v>
+        <v>0.763140667579433</v>
       </c>
       <c r="D7" t="n">
-        <v>0.638697250451824</v>
+        <v>0.780784036855754</v>
       </c>
       <c r="E7" t="n">
-        <v>0.835006156623799</v>
+        <v>0.866088097442708</v>
       </c>
       <c r="F7" t="n">
-        <v>0.946115214989885</v>
+        <v>0.693971325525491</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.826369426010633</v>
+        <v>0.623491556309587</v>
       </c>
       <c r="I7" t="n">
-        <v>0.866088097442708</v>
+        <v>0.614304469513975</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.866428171542027</v>
       </c>
     </row>
     <row r="8">
@@ -860,28 +943,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.724759269901657</v>
+        <v>0.438820638841603</v>
       </c>
       <c r="C8" t="n">
-        <v>0.825306777206141</v>
+        <v>0.722969574589664</v>
       </c>
       <c r="D8" t="n">
-        <v>0.44716708401268</v>
+        <v>0.708063599850068</v>
       </c>
       <c r="E8" t="n">
-        <v>0.729186065614364</v>
+        <v>0.767516242826121</v>
       </c>
       <c r="F8" t="n">
-        <v>0.727100492243932</v>
+        <v>0.686000509241168</v>
       </c>
       <c r="G8" t="n">
-        <v>0.826369426010633</v>
+        <v>0.623491556309587</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.693971325525491</v>
+        <v>0.991635911227623</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.767554265037877</v>
       </c>
     </row>
     <row r="9">
@@ -889,27 +975,62 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.764551818279103</v>
+        <v>0.424123380735669</v>
       </c>
       <c r="C9" t="n">
+        <v>0.733119324885382</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.692229881668236</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.769218318413894</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.71172756770144</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.614304469513975</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.991635911227623</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.769171997949829</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.638096956923035</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.835647840454511</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.945880995727681</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.999977186256954</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.825306777206141</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.866428171542027</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.476329863035688</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.763140667579433</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.780784036855754</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.866088097442708</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.693971325525491</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="H10" t="n">
+        <v>0.767554265037877</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.769171997949829</v>
+      </c>
+      <c r="J10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -955,6 +1076,9 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -964,25 +1088,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.653342754964692</v>
+        <v>0.901804218632853</v>
       </c>
       <c r="D2" t="n">
-        <v>0.909504651891034</v>
+        <v>0.356194649740909</v>
       </c>
       <c r="E2" t="n">
-        <v>0.998177204562645</v>
+        <v>0.435519780609543</v>
       </c>
       <c r="F2" t="n">
-        <v>0.484202971159519</v>
+        <v>0.458418296887294</v>
       </c>
       <c r="G2" t="n">
-        <v>0.623127722947945</v>
+        <v>0.733437290156057</v>
       </c>
       <c r="H2" t="n">
-        <v>0.588634783690962</v>
+        <v>0.806699412156276</v>
       </c>
       <c r="I2" t="n">
-        <v>0.880083858871079</v>
+        <v>0.829515381238252</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.462976500925549</v>
       </c>
     </row>
     <row r="3">
@@ -990,28 +1117,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.653342754964692</v>
+        <v>0.901804218632853</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.462976500925549</v>
+        <v>0.509983922154108</v>
       </c>
       <c r="E3" t="n">
+        <v>0.648756494372831</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.606206977827473</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.889843101802611</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.681576636415055</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.726771597449783</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.674230460908826</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.935855024521929</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.99612934757487</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.925827314057919</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.78801119700484</v>
       </c>
     </row>
     <row r="4">
@@ -1019,28 +1149,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.909504651891034</v>
+        <v>0.356194649740909</v>
       </c>
       <c r="C4" t="n">
-        <v>0.462976500925549</v>
+        <v>0.509983922154108</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.901804218632853</v>
+        <v>0.945919536392486</v>
       </c>
       <c r="F4" t="n">
-        <v>0.356194649740909</v>
+        <v>0.925148662955917</v>
       </c>
       <c r="G4" t="n">
-        <v>0.435519780609543</v>
+        <v>0.626115640850283</v>
       </c>
       <c r="H4" t="n">
-        <v>0.458418296887294</v>
+        <v>0.13812017166833</v>
       </c>
       <c r="I4" t="n">
-        <v>0.733437290156057</v>
+        <v>0.155712844922479</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.935855024521929</v>
       </c>
     </row>
     <row r="5">
@@ -1048,28 +1181,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.998177204562645</v>
+        <v>0.435519780609543</v>
       </c>
       <c r="C5" t="n">
-        <v>0.674230460908826</v>
+        <v>0.648756494372831</v>
       </c>
       <c r="D5" t="n">
-        <v>0.901804218632853</v>
+        <v>0.945919536392486</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.509983922154108</v>
+        <v>0.921162587247194</v>
       </c>
       <c r="G5" t="n">
-        <v>0.648756494372831</v>
+        <v>0.7706107038364</v>
       </c>
       <c r="H5" t="n">
-        <v>0.606206977827473</v>
+        <v>0.196686159916996</v>
       </c>
       <c r="I5" t="n">
-        <v>0.889843101802611</v>
+        <v>0.237231030273605</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.99612934757487</v>
       </c>
     </row>
     <row r="6">
@@ -1077,28 +1213,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.484202971159519</v>
+        <v>0.458418296887294</v>
       </c>
       <c r="C6" t="n">
-        <v>0.935855024521929</v>
+        <v>0.606206977827473</v>
       </c>
       <c r="D6" t="n">
-        <v>0.356194649740909</v>
+        <v>0.925148662955917</v>
       </c>
       <c r="E6" t="n">
-        <v>0.509983922154108</v>
+        <v>0.921162587247194</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.945919536392486</v>
+        <v>0.762835256792117</v>
       </c>
       <c r="H6" t="n">
-        <v>0.925148662955917</v>
+        <v>0.219368230834023</v>
       </c>
       <c r="I6" t="n">
-        <v>0.626115640850283</v>
+        <v>0.225653261515404</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.925827314057919</v>
       </c>
     </row>
     <row r="7">
@@ -1106,28 +1245,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.623127722947945</v>
+        <v>0.733437290156057</v>
       </c>
       <c r="C7" t="n">
-        <v>0.99612934757487</v>
+        <v>0.889843101802611</v>
       </c>
       <c r="D7" t="n">
-        <v>0.435519780609543</v>
+        <v>0.626115640850283</v>
       </c>
       <c r="E7" t="n">
-        <v>0.648756494372831</v>
+        <v>0.7706107038364</v>
       </c>
       <c r="F7" t="n">
-        <v>0.945919536392486</v>
+        <v>0.762835256792117</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.921162587247194</v>
+        <v>0.490274942033487</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7706107038364</v>
+        <v>0.531082419831071</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.78801119700484</v>
       </c>
     </row>
     <row r="8">
@@ -1135,28 +1277,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.588634783690962</v>
+        <v>0.806699412156276</v>
       </c>
       <c r="C8" t="n">
-        <v>0.925827314057919</v>
+        <v>0.681576636415055</v>
       </c>
       <c r="D8" t="n">
-        <v>0.458418296887294</v>
+        <v>0.13812017166833</v>
       </c>
       <c r="E8" t="n">
-        <v>0.606206977827473</v>
+        <v>0.196686159916996</v>
       </c>
       <c r="F8" t="n">
-        <v>0.925148662955917</v>
+        <v>0.219368230834023</v>
       </c>
       <c r="G8" t="n">
-        <v>0.921162587247194</v>
+        <v>0.490274942033487</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.762835256792117</v>
+        <v>0.990347129933348</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.217741007283888</v>
       </c>
     </row>
     <row r="9">
@@ -1164,27 +1309,62 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.880083858871079</v>
+        <v>0.829515381238252</v>
       </c>
       <c r="C9" t="n">
+        <v>0.726771597449783</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.155712844922479</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.237231030273605</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.225653261515404</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.531082419831071</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.990347129933348</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.257989742803437</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.462976500925549</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.674230460908826</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.935855024521929</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.99612934757487</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.925827314057919</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.78801119700484</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.733437290156057</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.889843101802611</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.626115640850283</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.7706107038364</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.762835256792117</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="H10" t="n">
+        <v>0.217741007283888</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.257989742803437</v>
+      </c>
+      <c r="J10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1230,6 +1410,9 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -1239,25 +1422,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.834389070974318</v>
+        <v>0.22339520763975</v>
       </c>
       <c r="D2" t="n">
-        <v>0.221918391528785</v>
+        <v>0.77372598741087</v>
       </c>
       <c r="E2" t="n">
-        <v>0.999768750645947</v>
+        <v>0.638697250451824</v>
       </c>
       <c r="F2" t="n">
-        <v>0.683402758279144</v>
+        <v>0.44716708401268</v>
       </c>
       <c r="G2" t="n">
-        <v>0.833683034767251</v>
+        <v>0.476329863035688</v>
       </c>
       <c r="H2" t="n">
-        <v>0.724759269901657</v>
+        <v>0.438820638841603</v>
       </c>
       <c r="I2" t="n">
-        <v>0.764551818279103</v>
+        <v>0.424123380735669</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.638096956923035</v>
       </c>
     </row>
     <row r="3">
@@ -1265,28 +1451,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.834389070974318</v>
+        <v>0.22339520763975</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.638096956923035</v>
+        <v>0.684885362084019</v>
       </c>
       <c r="E3" t="n">
+        <v>0.835006156623799</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.729186065614364</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.763140667579433</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.722969574589664</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.733119324885382</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.835647840454511</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.945880995727681</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.999977186256954</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.825306777206141</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.866428171542027</v>
       </c>
     </row>
     <row r="4">
@@ -1294,28 +1483,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.221918391528785</v>
+        <v>0.77372598741087</v>
       </c>
       <c r="C4" t="n">
-        <v>0.638096956923035</v>
+        <v>0.684885362084019</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.22339520763975</v>
+        <v>0.946115214989885</v>
       </c>
       <c r="F4" t="n">
-        <v>0.77372598741087</v>
+        <v>0.727100492243932</v>
       </c>
       <c r="G4" t="n">
-        <v>0.638697250451824</v>
+        <v>0.780784036855754</v>
       </c>
       <c r="H4" t="n">
-        <v>0.44716708401268</v>
+        <v>0.708063599850068</v>
       </c>
       <c r="I4" t="n">
-        <v>0.476329863035688</v>
+        <v>0.692229881668236</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.945880995727681</v>
       </c>
     </row>
     <row r="5">
@@ -1323,28 +1515,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.999768750645947</v>
+        <v>0.638697250451824</v>
       </c>
       <c r="C5" t="n">
-        <v>0.835647840454511</v>
+        <v>0.835006156623799</v>
       </c>
       <c r="D5" t="n">
-        <v>0.22339520763975</v>
+        <v>0.946115214989885</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.684885362084019</v>
+        <v>0.826369426010633</v>
       </c>
       <c r="G5" t="n">
-        <v>0.835006156623799</v>
+        <v>0.866088097442708</v>
       </c>
       <c r="H5" t="n">
-        <v>0.729186065614364</v>
+        <v>0.767516242826121</v>
       </c>
       <c r="I5" t="n">
-        <v>0.763140667579433</v>
+        <v>0.769218318413894</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.999977186256954</v>
       </c>
     </row>
     <row r="6">
@@ -1352,28 +1547,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.683402758279144</v>
+        <v>0.44716708401268</v>
       </c>
       <c r="C6" t="n">
-        <v>0.945880995727681</v>
+        <v>0.729186065614364</v>
       </c>
       <c r="D6" t="n">
-        <v>0.77372598741087</v>
+        <v>0.727100492243932</v>
       </c>
       <c r="E6" t="n">
-        <v>0.684885362084019</v>
+        <v>0.826369426010633</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.946115214989885</v>
+        <v>0.693971325525491</v>
       </c>
       <c r="H6" t="n">
-        <v>0.727100492243932</v>
+        <v>0.686000509241168</v>
       </c>
       <c r="I6" t="n">
-        <v>0.780784036855754</v>
+        <v>0.71172756770144</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.825306777206141</v>
       </c>
     </row>
     <row r="7">
@@ -1381,28 +1579,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.833683034767251</v>
+        <v>0.476329863035688</v>
       </c>
       <c r="C7" t="n">
-        <v>0.999977186256954</v>
+        <v>0.763140667579433</v>
       </c>
       <c r="D7" t="n">
-        <v>0.638697250451824</v>
+        <v>0.780784036855754</v>
       </c>
       <c r="E7" t="n">
-        <v>0.835006156623799</v>
+        <v>0.866088097442708</v>
       </c>
       <c r="F7" t="n">
-        <v>0.946115214989885</v>
+        <v>0.693971325525491</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.826369426010633</v>
+        <v>0.623491556309587</v>
       </c>
       <c r="I7" t="n">
-        <v>0.866088097442708</v>
+        <v>0.614304469513975</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.866428171542027</v>
       </c>
     </row>
     <row r="8">
@@ -1410,28 +1611,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.724759269901657</v>
+        <v>0.438820638841603</v>
       </c>
       <c r="C8" t="n">
-        <v>0.825306777206141</v>
+        <v>0.722969574589664</v>
       </c>
       <c r="D8" t="n">
-        <v>0.44716708401268</v>
+        <v>0.708063599850068</v>
       </c>
       <c r="E8" t="n">
-        <v>0.729186065614364</v>
+        <v>0.767516242826121</v>
       </c>
       <c r="F8" t="n">
-        <v>0.727100492243932</v>
+        <v>0.686000509241168</v>
       </c>
       <c r="G8" t="n">
-        <v>0.826369426010633</v>
+        <v>0.623491556309587</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.693971325525491</v>
+        <v>0.991635911227623</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.767554265037877</v>
       </c>
     </row>
     <row r="9">
@@ -1439,27 +1643,62 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.764551818279103</v>
+        <v>0.424123380735669</v>
       </c>
       <c r="C9" t="n">
+        <v>0.733119324885382</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.692229881668236</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.769218318413894</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.71172756770144</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.614304469513975</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.991635911227623</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.769171997949829</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.638096956923035</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.835647840454511</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.945880995727681</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.999977186256954</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.825306777206141</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.866428171542027</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.476329863035688</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.763140667579433</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.780784036855754</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.866088097442708</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.693971325525491</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="H10" t="n">
+        <v>0.767554265037877</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.769171997949829</v>
+      </c>
+      <c r="J10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1505,6 +1744,9 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -1514,25 +1756,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.653342754964692</v>
+        <v>0.901804218632853</v>
       </c>
       <c r="D2" t="n">
-        <v>0.909504651891034</v>
+        <v>0.356194649740909</v>
       </c>
       <c r="E2" t="n">
-        <v>0.998177204562645</v>
+        <v>0.435519780609543</v>
       </c>
       <c r="F2" t="n">
-        <v>0.484202971159519</v>
+        <v>0.458418296887294</v>
       </c>
       <c r="G2" t="n">
-        <v>0.623127722947945</v>
+        <v>0.733437290156057</v>
       </c>
       <c r="H2" t="n">
-        <v>0.588634783690962</v>
+        <v>0.806699412156276</v>
       </c>
       <c r="I2" t="n">
-        <v>0.880083858871079</v>
+        <v>0.829515381238252</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.462976500925549</v>
       </c>
     </row>
     <row r="3">
@@ -1540,28 +1785,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.653342754964692</v>
+        <v>0.901804218632853</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.462976500925549</v>
+        <v>0.509983922154108</v>
       </c>
       <c r="E3" t="n">
+        <v>0.648756494372831</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.606206977827473</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.889843101802611</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.681576636415055</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.726771597449783</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.674230460908826</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.935855024521929</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.99612934757487</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.925827314057919</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.78801119700484</v>
       </c>
     </row>
     <row r="4">
@@ -1569,28 +1817,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.909504651891034</v>
+        <v>0.356194649740909</v>
       </c>
       <c r="C4" t="n">
-        <v>0.462976500925549</v>
+        <v>0.509983922154108</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.901804218632853</v>
+        <v>0.945919536392486</v>
       </c>
       <c r="F4" t="n">
-        <v>0.356194649740909</v>
+        <v>0.925148662955917</v>
       </c>
       <c r="G4" t="n">
-        <v>0.435519780609543</v>
+        <v>0.626115640850283</v>
       </c>
       <c r="H4" t="n">
-        <v>0.458418296887294</v>
+        <v>0.13812017166833</v>
       </c>
       <c r="I4" t="n">
-        <v>0.733437290156057</v>
+        <v>0.155712844922479</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.935855024521929</v>
       </c>
     </row>
     <row r="5">
@@ -1598,28 +1849,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.998177204562645</v>
+        <v>0.435519780609543</v>
       </c>
       <c r="C5" t="n">
-        <v>0.674230460908826</v>
+        <v>0.648756494372831</v>
       </c>
       <c r="D5" t="n">
-        <v>0.901804218632853</v>
+        <v>0.945919536392486</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.509983922154108</v>
+        <v>0.921162587247194</v>
       </c>
       <c r="G5" t="n">
-        <v>0.648756494372831</v>
+        <v>0.7706107038364</v>
       </c>
       <c r="H5" t="n">
-        <v>0.606206977827473</v>
+        <v>0.196686159916996</v>
       </c>
       <c r="I5" t="n">
-        <v>0.889843101802611</v>
+        <v>0.237231030273605</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.99612934757487</v>
       </c>
     </row>
     <row r="6">
@@ -1627,28 +1881,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.484202971159519</v>
+        <v>0.458418296887294</v>
       </c>
       <c r="C6" t="n">
-        <v>0.935855024521929</v>
+        <v>0.606206977827473</v>
       </c>
       <c r="D6" t="n">
-        <v>0.356194649740909</v>
+        <v>0.925148662955917</v>
       </c>
       <c r="E6" t="n">
-        <v>0.509983922154108</v>
+        <v>0.921162587247194</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.945919536392486</v>
+        <v>0.762835256792117</v>
       </c>
       <c r="H6" t="n">
-        <v>0.925148662955917</v>
+        <v>0.219368230834023</v>
       </c>
       <c r="I6" t="n">
-        <v>0.626115640850283</v>
+        <v>0.225653261515404</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.925827314057919</v>
       </c>
     </row>
     <row r="7">
@@ -1656,28 +1913,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.623127722947945</v>
+        <v>0.733437290156057</v>
       </c>
       <c r="C7" t="n">
-        <v>0.99612934757487</v>
+        <v>0.889843101802611</v>
       </c>
       <c r="D7" t="n">
-        <v>0.435519780609543</v>
+        <v>0.626115640850283</v>
       </c>
       <c r="E7" t="n">
-        <v>0.648756494372831</v>
+        <v>0.7706107038364</v>
       </c>
       <c r="F7" t="n">
-        <v>0.945919536392486</v>
+        <v>0.762835256792117</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.921162587247194</v>
+        <v>0.490274942033487</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7706107038364</v>
+        <v>0.531082419831071</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.78801119700484</v>
       </c>
     </row>
     <row r="8">
@@ -1685,28 +1945,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.588634783690962</v>
+        <v>0.806699412156276</v>
       </c>
       <c r="C8" t="n">
-        <v>0.925827314057919</v>
+        <v>0.681576636415055</v>
       </c>
       <c r="D8" t="n">
-        <v>0.458418296887294</v>
+        <v>0.13812017166833</v>
       </c>
       <c r="E8" t="n">
-        <v>0.606206977827473</v>
+        <v>0.196686159916996</v>
       </c>
       <c r="F8" t="n">
-        <v>0.925148662955917</v>
+        <v>0.219368230834023</v>
       </c>
       <c r="G8" t="n">
-        <v>0.921162587247194</v>
+        <v>0.490274942033487</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.762835256792117</v>
+        <v>0.990347129933348</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.217741007283888</v>
       </c>
     </row>
     <row r="9">
@@ -1714,27 +1977,62 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.880083858871079</v>
+        <v>0.829515381238252</v>
       </c>
       <c r="C9" t="n">
+        <v>0.726771597449783</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.155712844922479</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.237231030273605</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.225653261515404</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.531082419831071</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.990347129933348</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.257989742803437</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.462976500925549</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.674230460908826</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.935855024521929</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.99612934757487</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.925827314057919</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.78801119700484</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.733437290156057</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.889843101802611</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.626115640850283</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.7706107038364</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.762835256792117</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="H10" t="n">
+        <v>0.217741007283888</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.257989742803437</v>
+      </c>
+      <c r="J10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1780,6 +2078,9 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -1789,25 +2090,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.834389070974318</v>
+        <v>0.22339520763975</v>
       </c>
       <c r="D2" t="n">
-        <v>0.221918391528785</v>
+        <v>0.77372598741087</v>
       </c>
       <c r="E2" t="n">
-        <v>0.999768750645947</v>
+        <v>0.638697250451824</v>
       </c>
       <c r="F2" t="n">
-        <v>0.683402758279144</v>
+        <v>0.44716708401268</v>
       </c>
       <c r="G2" t="n">
-        <v>0.833683034767251</v>
+        <v>0.476329863035688</v>
       </c>
       <c r="H2" t="n">
-        <v>0.724759269901657</v>
+        <v>0.438820638841603</v>
       </c>
       <c r="I2" t="n">
-        <v>0.764551818279103</v>
+        <v>0.424123380735669</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.638096956923035</v>
       </c>
     </row>
     <row r="3">
@@ -1815,28 +2119,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.834389070974318</v>
+        <v>0.22339520763975</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.638096956923035</v>
+        <v>0.684885362084019</v>
       </c>
       <c r="E3" t="n">
+        <v>0.835006156623799</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.729186065614364</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.763140667579433</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.722969574589664</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.733119324885382</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.835647840454511</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.945880995727681</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.999977186256954</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.825306777206141</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.866428171542027</v>
       </c>
     </row>
     <row r="4">
@@ -1844,28 +2151,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.221918391528785</v>
+        <v>0.77372598741087</v>
       </c>
       <c r="C4" t="n">
-        <v>0.638096956923035</v>
+        <v>0.684885362084019</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.22339520763975</v>
+        <v>0.946115214989885</v>
       </c>
       <c r="F4" t="n">
-        <v>0.77372598741087</v>
+        <v>0.727100492243932</v>
       </c>
       <c r="G4" t="n">
-        <v>0.638697250451824</v>
+        <v>0.780784036855754</v>
       </c>
       <c r="H4" t="n">
-        <v>0.44716708401268</v>
+        <v>0.708063599850068</v>
       </c>
       <c r="I4" t="n">
-        <v>0.476329863035688</v>
+        <v>0.692229881668236</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.945880995727681</v>
       </c>
     </row>
     <row r="5">
@@ -1873,28 +2183,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.999768750645947</v>
+        <v>0.638697250451824</v>
       </c>
       <c r="C5" t="n">
-        <v>0.835647840454511</v>
+        <v>0.835006156623799</v>
       </c>
       <c r="D5" t="n">
-        <v>0.22339520763975</v>
+        <v>0.946115214989885</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.684885362084019</v>
+        <v>0.826369426010633</v>
       </c>
       <c r="G5" t="n">
-        <v>0.835006156623799</v>
+        <v>0.866088097442708</v>
       </c>
       <c r="H5" t="n">
-        <v>0.729186065614364</v>
+        <v>0.767516242826121</v>
       </c>
       <c r="I5" t="n">
-        <v>0.763140667579433</v>
+        <v>0.769218318413894</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.999977186256954</v>
       </c>
     </row>
     <row r="6">
@@ -1902,28 +2215,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.683402758279144</v>
+        <v>0.44716708401268</v>
       </c>
       <c r="C6" t="n">
-        <v>0.945880995727681</v>
+        <v>0.729186065614364</v>
       </c>
       <c r="D6" t="n">
-        <v>0.77372598741087</v>
+        <v>0.727100492243932</v>
       </c>
       <c r="E6" t="n">
-        <v>0.684885362084019</v>
+        <v>0.826369426010633</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.946115214989885</v>
+        <v>0.693971325525491</v>
       </c>
       <c r="H6" t="n">
-        <v>0.727100492243932</v>
+        <v>0.686000509241168</v>
       </c>
       <c r="I6" t="n">
-        <v>0.780784036855754</v>
+        <v>0.71172756770144</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.825306777206141</v>
       </c>
     </row>
     <row r="7">
@@ -1931,28 +2247,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.833683034767251</v>
+        <v>0.476329863035688</v>
       </c>
       <c r="C7" t="n">
-        <v>0.999977186256954</v>
+        <v>0.763140667579433</v>
       </c>
       <c r="D7" t="n">
-        <v>0.638697250451824</v>
+        <v>0.780784036855754</v>
       </c>
       <c r="E7" t="n">
-        <v>0.835006156623799</v>
+        <v>0.866088097442708</v>
       </c>
       <c r="F7" t="n">
-        <v>0.946115214989885</v>
+        <v>0.693971325525491</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.826369426010633</v>
+        <v>0.623491556309587</v>
       </c>
       <c r="I7" t="n">
-        <v>0.866088097442708</v>
+        <v>0.614304469513975</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.866428171542027</v>
       </c>
     </row>
     <row r="8">
@@ -1960,28 +2279,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.724759269901657</v>
+        <v>0.438820638841603</v>
       </c>
       <c r="C8" t="n">
-        <v>0.825306777206141</v>
+        <v>0.722969574589664</v>
       </c>
       <c r="D8" t="n">
-        <v>0.44716708401268</v>
+        <v>0.708063599850068</v>
       </c>
       <c r="E8" t="n">
-        <v>0.729186065614364</v>
+        <v>0.767516242826121</v>
       </c>
       <c r="F8" t="n">
-        <v>0.727100492243932</v>
+        <v>0.686000509241168</v>
       </c>
       <c r="G8" t="n">
-        <v>0.826369426010633</v>
+        <v>0.623491556309587</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.693971325525491</v>
+        <v>0.991635911227623</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.767554265037877</v>
       </c>
     </row>
     <row r="9">
@@ -1989,27 +2311,62 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.764551818279103</v>
+        <v>0.424123380735669</v>
       </c>
       <c r="C9" t="n">
+        <v>0.733119324885382</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.692229881668236</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.769218318413894</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.71172756770144</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.614304469513975</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.991635911227623</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.769171997949829</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.638096956923035</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.835647840454511</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.945880995727681</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.999977186256954</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.825306777206141</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.866428171542027</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.476329863035688</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.763140667579433</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.780784036855754</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.866088097442708</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.693971325525491</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="H10" t="n">
+        <v>0.767554265037877</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.769171997949829</v>
+      </c>
+      <c r="J10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2055,6 +2412,9 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -2064,25 +2424,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.653342754964692</v>
+        <v>0.901804218632853</v>
       </c>
       <c r="D2" t="n">
-        <v>0.909504651891034</v>
+        <v>0.356194649740909</v>
       </c>
       <c r="E2" t="n">
-        <v>0.998177204562645</v>
+        <v>0.435519780609543</v>
       </c>
       <c r="F2" t="n">
-        <v>0.484202971159519</v>
+        <v>0.458418296887294</v>
       </c>
       <c r="G2" t="n">
-        <v>0.623127722947945</v>
+        <v>0.733437290156057</v>
       </c>
       <c r="H2" t="n">
-        <v>0.588634783690962</v>
+        <v>0.806699412156276</v>
       </c>
       <c r="I2" t="n">
-        <v>0.880083858871079</v>
+        <v>0.829515381238252</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.462976500925549</v>
       </c>
     </row>
     <row r="3">
@@ -2090,28 +2453,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.653342754964692</v>
+        <v>0.901804218632853</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.462976500925549</v>
+        <v>0.509983922154108</v>
       </c>
       <c r="E3" t="n">
+        <v>0.648756494372831</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.606206977827473</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.889843101802611</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.681576636415055</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.726771597449783</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.674230460908826</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.935855024521929</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.99612934757487</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.925827314057919</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.78801119700484</v>
       </c>
     </row>
     <row r="4">
@@ -2119,28 +2485,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.909504651891034</v>
+        <v>0.356194649740909</v>
       </c>
       <c r="C4" t="n">
-        <v>0.462976500925549</v>
+        <v>0.509983922154108</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.901804218632853</v>
+        <v>0.945919536392486</v>
       </c>
       <c r="F4" t="n">
-        <v>0.356194649740909</v>
+        <v>0.925148662955917</v>
       </c>
       <c r="G4" t="n">
-        <v>0.435519780609543</v>
+        <v>0.626115640850283</v>
       </c>
       <c r="H4" t="n">
-        <v>0.458418296887294</v>
+        <v>0.13812017166833</v>
       </c>
       <c r="I4" t="n">
-        <v>0.733437290156057</v>
+        <v>0.155712844922479</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.935855024521929</v>
       </c>
     </row>
     <row r="5">
@@ -2148,28 +2517,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.998177204562645</v>
+        <v>0.435519780609543</v>
       </c>
       <c r="C5" t="n">
-        <v>0.674230460908826</v>
+        <v>0.648756494372831</v>
       </c>
       <c r="D5" t="n">
-        <v>0.901804218632853</v>
+        <v>0.945919536392486</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.509983922154108</v>
+        <v>0.921162587247194</v>
       </c>
       <c r="G5" t="n">
-        <v>0.648756494372831</v>
+        <v>0.7706107038364</v>
       </c>
       <c r="H5" t="n">
-        <v>0.606206977827473</v>
+        <v>0.196686159916996</v>
       </c>
       <c r="I5" t="n">
-        <v>0.889843101802611</v>
+        <v>0.237231030273605</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.99612934757487</v>
       </c>
     </row>
     <row r="6">
@@ -2177,28 +2549,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.484202971159519</v>
+        <v>0.458418296887294</v>
       </c>
       <c r="C6" t="n">
-        <v>0.935855024521929</v>
+        <v>0.606206977827473</v>
       </c>
       <c r="D6" t="n">
-        <v>0.356194649740909</v>
+        <v>0.925148662955917</v>
       </c>
       <c r="E6" t="n">
-        <v>0.509983922154108</v>
+        <v>0.921162587247194</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.945919536392486</v>
+        <v>0.762835256792117</v>
       </c>
       <c r="H6" t="n">
-        <v>0.925148662955917</v>
+        <v>0.219368230834023</v>
       </c>
       <c r="I6" t="n">
-        <v>0.626115640850283</v>
+        <v>0.225653261515404</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.925827314057919</v>
       </c>
     </row>
     <row r="7">
@@ -2206,28 +2581,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.623127722947945</v>
+        <v>0.733437290156057</v>
       </c>
       <c r="C7" t="n">
-        <v>0.99612934757487</v>
+        <v>0.889843101802611</v>
       </c>
       <c r="D7" t="n">
-        <v>0.435519780609543</v>
+        <v>0.626115640850283</v>
       </c>
       <c r="E7" t="n">
-        <v>0.648756494372831</v>
+        <v>0.7706107038364</v>
       </c>
       <c r="F7" t="n">
-        <v>0.945919536392486</v>
+        <v>0.762835256792117</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.921162587247194</v>
+        <v>0.490274942033487</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7706107038364</v>
+        <v>0.531082419831071</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.78801119700484</v>
       </c>
     </row>
     <row r="8">
@@ -2235,28 +2613,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.588634783690962</v>
+        <v>0.806699412156276</v>
       </c>
       <c r="C8" t="n">
-        <v>0.925827314057919</v>
+        <v>0.681576636415055</v>
       </c>
       <c r="D8" t="n">
-        <v>0.458418296887294</v>
+        <v>0.13812017166833</v>
       </c>
       <c r="E8" t="n">
-        <v>0.606206977827473</v>
+        <v>0.196686159916996</v>
       </c>
       <c r="F8" t="n">
-        <v>0.925148662955917</v>
+        <v>0.219368230834023</v>
       </c>
       <c r="G8" t="n">
-        <v>0.921162587247194</v>
+        <v>0.490274942033487</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.762835256792117</v>
+        <v>0.990347129933348</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.217741007283888</v>
       </c>
     </row>
     <row r="9">
@@ -2264,27 +2645,62 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.880083858871079</v>
+        <v>0.829515381238252</v>
       </c>
       <c r="C9" t="n">
+        <v>0.726771597449783</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.155712844922479</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.237231030273605</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.225653261515404</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.531082419831071</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.990347129933348</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.257989742803437</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.462976500925549</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.674230460908826</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.935855024521929</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.99612934757487</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.925827314057919</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.78801119700484</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.733437290156057</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.889843101802611</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.626115640850283</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.7706107038364</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.762835256792117</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="H10" t="n">
+        <v>0.217741007283888</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.257989742803437</v>
+      </c>
+      <c r="J10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2330,6 +2746,9 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -2339,25 +2758,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.834389070974318</v>
+        <v>0.22339520763975</v>
       </c>
       <c r="D2" t="n">
-        <v>0.221918391528785</v>
+        <v>0.77372598741087</v>
       </c>
       <c r="E2" t="n">
-        <v>0.999768750645947</v>
+        <v>0.638697250451824</v>
       </c>
       <c r="F2" t="n">
-        <v>0.683402758279144</v>
+        <v>0.44716708401268</v>
       </c>
       <c r="G2" t="n">
-        <v>0.833683034767251</v>
+        <v>0.476329863035688</v>
       </c>
       <c r="H2" t="n">
-        <v>0.724759269901657</v>
+        <v>0.438820638841603</v>
       </c>
       <c r="I2" t="n">
-        <v>0.764551818279103</v>
+        <v>0.424123380735669</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.638096956923035</v>
       </c>
     </row>
     <row r="3">
@@ -2365,28 +2787,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.834389070974318</v>
+        <v>0.22339520763975</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.638096956923035</v>
+        <v>0.684885362084019</v>
       </c>
       <c r="E3" t="n">
+        <v>0.835006156623799</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.729186065614364</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.763140667579433</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.722969574589664</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.733119324885382</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.835647840454511</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.945880995727681</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.999977186256954</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.825306777206141</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.866428171542027</v>
       </c>
     </row>
     <row r="4">
@@ -2394,28 +2819,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.221918391528785</v>
+        <v>0.77372598741087</v>
       </c>
       <c r="C4" t="n">
-        <v>0.638096956923035</v>
+        <v>0.684885362084019</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.22339520763975</v>
+        <v>0.946115214989885</v>
       </c>
       <c r="F4" t="n">
-        <v>0.77372598741087</v>
+        <v>0.727100492243932</v>
       </c>
       <c r="G4" t="n">
-        <v>0.638697250451824</v>
+        <v>0.780784036855754</v>
       </c>
       <c r="H4" t="n">
-        <v>0.44716708401268</v>
+        <v>0.708063599850068</v>
       </c>
       <c r="I4" t="n">
-        <v>0.476329863035688</v>
+        <v>0.692229881668236</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.945880995727681</v>
       </c>
     </row>
     <row r="5">
@@ -2423,28 +2851,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.999768750645947</v>
+        <v>0.638697250451824</v>
       </c>
       <c r="C5" t="n">
-        <v>0.835647840454511</v>
+        <v>0.835006156623799</v>
       </c>
       <c r="D5" t="n">
-        <v>0.22339520763975</v>
+        <v>0.946115214989885</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.684885362084019</v>
+        <v>0.826369426010633</v>
       </c>
       <c r="G5" t="n">
-        <v>0.835006156623799</v>
+        <v>0.866088097442708</v>
       </c>
       <c r="H5" t="n">
-        <v>0.729186065614364</v>
+        <v>0.767516242826121</v>
       </c>
       <c r="I5" t="n">
-        <v>0.763140667579433</v>
+        <v>0.769218318413894</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.999977186256954</v>
       </c>
     </row>
     <row r="6">
@@ -2452,28 +2883,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.683402758279144</v>
+        <v>0.44716708401268</v>
       </c>
       <c r="C6" t="n">
-        <v>0.945880995727681</v>
+        <v>0.729186065614364</v>
       </c>
       <c r="D6" t="n">
-        <v>0.77372598741087</v>
+        <v>0.727100492243932</v>
       </c>
       <c r="E6" t="n">
-        <v>0.684885362084019</v>
+        <v>0.826369426010633</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.946115214989885</v>
+        <v>0.693971325525491</v>
       </c>
       <c r="H6" t="n">
-        <v>0.727100492243932</v>
+        <v>0.686000509241168</v>
       </c>
       <c r="I6" t="n">
-        <v>0.780784036855754</v>
+        <v>0.71172756770144</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.825306777206141</v>
       </c>
     </row>
     <row r="7">
@@ -2481,28 +2915,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.833683034767251</v>
+        <v>0.476329863035688</v>
       </c>
       <c r="C7" t="n">
-        <v>0.999977186256954</v>
+        <v>0.763140667579433</v>
       </c>
       <c r="D7" t="n">
-        <v>0.638697250451824</v>
+        <v>0.780784036855754</v>
       </c>
       <c r="E7" t="n">
-        <v>0.835006156623799</v>
+        <v>0.866088097442708</v>
       </c>
       <c r="F7" t="n">
-        <v>0.946115214989885</v>
+        <v>0.693971325525491</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.826369426010633</v>
+        <v>0.623491556309587</v>
       </c>
       <c r="I7" t="n">
-        <v>0.866088097442708</v>
+        <v>0.614304469513975</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.866428171542027</v>
       </c>
     </row>
     <row r="8">
@@ -2510,28 +2947,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.724759269901657</v>
+        <v>0.438820638841603</v>
       </c>
       <c r="C8" t="n">
-        <v>0.825306777206141</v>
+        <v>0.722969574589664</v>
       </c>
       <c r="D8" t="n">
-        <v>0.44716708401268</v>
+        <v>0.708063599850068</v>
       </c>
       <c r="E8" t="n">
-        <v>0.729186065614364</v>
+        <v>0.767516242826121</v>
       </c>
       <c r="F8" t="n">
-        <v>0.727100492243932</v>
+        <v>0.686000509241168</v>
       </c>
       <c r="G8" t="n">
-        <v>0.826369426010633</v>
+        <v>0.623491556309587</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.693971325525491</v>
+        <v>0.991635911227623</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.767554265037877</v>
       </c>
     </row>
     <row r="9">
@@ -2539,27 +2979,62 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.764551818279103</v>
+        <v>0.424123380735669</v>
       </c>
       <c r="C9" t="n">
+        <v>0.733119324885382</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.692229881668236</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.769218318413894</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.71172756770144</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.614304469513975</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.991635911227623</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.769171997949829</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.638096956923035</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.835647840454511</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.945880995727681</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.999977186256954</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.825306777206141</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.866428171542027</v>
       </c>
-      <c r="D9" t="n">
-        <v>0.476329863035688</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.763140667579433</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.780784036855754</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.866088097442708</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.693971325525491</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="H10" t="n">
+        <v>0.767554265037877</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.769171997949829</v>
+      </c>
+      <c r="J10" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise à jour des indices avec la valeur de l'argent
</commit_message>
<xml_diff>
--- a/scripts/Edouard/Correlation_matrix.xlsx
+++ b/scripts/Edouard/Correlation_matrix.xlsx
@@ -424,7 +424,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.842917893904185</v>
+        <v>0.842917893904186</v>
       </c>
       <c r="D2" t="n">
         <v>0.958996668783352</v>
@@ -442,10 +442,10 @@
         <v>0.962767579167416</v>
       </c>
       <c r="I2" t="n">
-        <v>0.371164058836417</v>
+        <v>0.371164058836418</v>
       </c>
       <c r="J2" t="n">
-        <v>0.534850797035608</v>
+        <v>0.508607244640602</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.842917893904185</v>
+        <v>0.842917893904186</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -462,22 +462,22 @@
         <v>0.785765468303247</v>
       </c>
       <c r="E3" t="n">
-        <v>0.824592179212595</v>
+        <v>0.824592179212594</v>
       </c>
       <c r="F3" t="n">
         <v>0.841204867324044</v>
       </c>
       <c r="G3" t="n">
-        <v>0.824209696684532</v>
+        <v>0.824209696684533</v>
       </c>
       <c r="H3" t="n">
         <v>0.830799138085553</v>
       </c>
       <c r="I3" t="n">
-        <v>0.313582679559778</v>
+        <v>0.31358267955978</v>
       </c>
       <c r="J3" t="n">
-        <v>0.458086604262501</v>
+        <v>0.434650836635204</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +494,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.940438981865428</v>
+        <v>0.940438981865429</v>
       </c>
       <c r="F4" t="n">
         <v>0.956814118369311</v>
@@ -506,10 +506,10 @@
         <v>0.920395539068851</v>
       </c>
       <c r="I4" t="n">
-        <v>0.448772691491425</v>
+        <v>0.448772691491427</v>
       </c>
       <c r="J4" t="n">
-        <v>0.588091319902675</v>
+        <v>0.570635046121742</v>
       </c>
     </row>
     <row r="5">
@@ -520,10 +520,10 @@
         <v>0.967125633214101</v>
       </c>
       <c r="C5" t="n">
-        <v>0.824592179212595</v>
+        <v>0.824592179212594</v>
       </c>
       <c r="D5" t="n">
-        <v>0.940438981865428</v>
+        <v>0.940438981865429</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -541,7 +541,7 @@
         <v>0.447592023877605</v>
       </c>
       <c r="J5" t="n">
-        <v>0.587092871672864</v>
+        <v>0.56686465844382</v>
       </c>
     </row>
     <row r="6">
@@ -570,10 +570,10 @@
         <v>0.963377815327466</v>
       </c>
       <c r="I6" t="n">
-        <v>0.366216660154031</v>
+        <v>0.366216660154032</v>
       </c>
       <c r="J6" t="n">
-        <v>0.530426115801221</v>
+        <v>0.503978676628744</v>
       </c>
     </row>
     <row r="7">
@@ -584,7 +584,7 @@
         <v>0.978840228886755</v>
       </c>
       <c r="C7" t="n">
-        <v>0.824209696684532</v>
+        <v>0.824209696684533</v>
       </c>
       <c r="D7" t="n">
         <v>0.960505640617623</v>
@@ -602,10 +602,10 @@
         <v>0.955386928907585</v>
       </c>
       <c r="I7" t="n">
-        <v>0.429574044433895</v>
+        <v>0.429574044433897</v>
       </c>
       <c r="J7" t="n">
-        <v>0.569501026842401</v>
+        <v>0.548295929369843</v>
       </c>
     </row>
     <row r="8">
@@ -637,7 +637,7 @@
         <v>0.447707609553343</v>
       </c>
       <c r="J8" t="n">
-        <v>0.586835717512416</v>
+        <v>0.562988208669169</v>
       </c>
     </row>
     <row r="9">
@@ -645,22 +645,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.371164058836417</v>
+        <v>0.371164058836418</v>
       </c>
       <c r="C9" t="n">
-        <v>0.313582679559778</v>
+        <v>0.31358267955978</v>
       </c>
       <c r="D9" t="n">
-        <v>0.448772691491425</v>
+        <v>0.448772691491427</v>
       </c>
       <c r="E9" t="n">
         <v>0.447592023877605</v>
       </c>
       <c r="F9" t="n">
-        <v>0.366216660154031</v>
+        <v>0.366216660154032</v>
       </c>
       <c r="G9" t="n">
-        <v>0.429574044433895</v>
+        <v>0.429574044433897</v>
       </c>
       <c r="H9" t="n">
         <v>0.447707609553343</v>
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.975842981424642</v>
+        <v>0.982398989941155</v>
       </c>
     </row>
     <row r="10">
@@ -677,28 +677,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.534850797035608</v>
+        <v>0.508607244640602</v>
       </c>
       <c r="C10" t="n">
-        <v>0.458086604262501</v>
+        <v>0.434650836635204</v>
       </c>
       <c r="D10" t="n">
-        <v>0.588091319902675</v>
+        <v>0.570635046121742</v>
       </c>
       <c r="E10" t="n">
-        <v>0.587092871672864</v>
+        <v>0.56686465844382</v>
       </c>
       <c r="F10" t="n">
-        <v>0.530426115801221</v>
+        <v>0.503978676628744</v>
       </c>
       <c r="G10" t="n">
-        <v>0.569501026842401</v>
+        <v>0.548295929369843</v>
       </c>
       <c r="H10" t="n">
-        <v>0.586835717512416</v>
+        <v>0.562988208669169</v>
       </c>
       <c r="I10" t="n">
-        <v>0.975842981424642</v>
+        <v>0.982398989941155</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -770,16 +770,16 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.734059818145422</v>
+        <v>0.734059818145425</v>
       </c>
       <c r="H2" t="n">
         <v>0.793058405988805</v>
       </c>
       <c r="I2" t="n">
-        <v>0.630564390054005</v>
+        <v>0.630564390054006</v>
       </c>
       <c r="J2" t="n">
-        <v>0.651273032242981</v>
+        <v>0.648210257109439</v>
       </c>
     </row>
     <row r="3">
@@ -802,16 +802,16 @@
         <v>0.953287974690855</v>
       </c>
       <c r="G3" t="n">
-        <v>0.697714256008796</v>
+        <v>0.697714256008798</v>
       </c>
       <c r="H3" t="n">
         <v>0.799159938782956</v>
       </c>
       <c r="I3" t="n">
-        <v>0.682018896940296</v>
+        <v>0.682018896940297</v>
       </c>
       <c r="J3" t="n">
-        <v>0.703225805637433</v>
+        <v>0.704670473081782</v>
       </c>
     </row>
     <row r="4">
@@ -840,10 +840,10 @@
         <v>0.622244230603934</v>
       </c>
       <c r="I4" t="n">
-        <v>0.59483180202416</v>
+        <v>0.594831802024161</v>
       </c>
       <c r="J4" t="n">
-        <v>0.588465941480315</v>
+        <v>0.584544350048525</v>
       </c>
     </row>
     <row r="5">
@@ -866,16 +866,16 @@
         <v>0.906346986391587</v>
       </c>
       <c r="G5" t="n">
-        <v>0.516908505069617</v>
+        <v>0.516908505069619</v>
       </c>
       <c r="H5" t="n">
-        <v>0.591426657035815</v>
+        <v>0.591426657035814</v>
       </c>
       <c r="I5" t="n">
-        <v>0.655976023165188</v>
+        <v>0.65597602316519</v>
       </c>
       <c r="J5" t="n">
-        <v>0.656353425734274</v>
+        <v>0.65341028409551</v>
       </c>
     </row>
     <row r="6">
@@ -898,16 +898,16 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.734059818145422</v>
+        <v>0.734059818145425</v>
       </c>
       <c r="H6" t="n">
         <v>0.793058405988805</v>
       </c>
       <c r="I6" t="n">
-        <v>0.630564390054005</v>
+        <v>0.630564390054006</v>
       </c>
       <c r="J6" t="n">
-        <v>0.651273032242981</v>
+        <v>0.648210257109439</v>
       </c>
     </row>
     <row r="7">
@@ -915,31 +915,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.734059818145422</v>
+        <v>0.734059818145425</v>
       </c>
       <c r="C7" t="n">
-        <v>0.697714256008796</v>
+        <v>0.697714256008798</v>
       </c>
       <c r="D7" t="n">
         <v>0.595677204446953</v>
       </c>
       <c r="E7" t="n">
-        <v>0.516908505069617</v>
+        <v>0.516908505069619</v>
       </c>
       <c r="F7" t="n">
-        <v>0.734059818145422</v>
+        <v>0.734059818145425</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.681847872154103</v>
+        <v>0.681847872154104</v>
       </c>
       <c r="I7" t="n">
-        <v>0.310905162143498</v>
+        <v>0.310905162143499</v>
       </c>
       <c r="J7" t="n">
-        <v>0.31460310234753</v>
+        <v>0.312714475422796</v>
       </c>
     </row>
     <row r="8">
@@ -956,13 +956,13 @@
         <v>0.622244230603934</v>
       </c>
       <c r="E8" t="n">
-        <v>0.591426657035815</v>
+        <v>0.591426657035814</v>
       </c>
       <c r="F8" t="n">
         <v>0.793058405988805</v>
       </c>
       <c r="G8" t="n">
-        <v>0.681847872154103</v>
+        <v>0.681847872154104</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
@@ -971,7 +971,7 @@
         <v>0.501737112321151</v>
       </c>
       <c r="J8" t="n">
-        <v>0.512194996299063</v>
+        <v>0.514036263994266</v>
       </c>
     </row>
     <row r="9">
@@ -979,22 +979,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.630564390054005</v>
+        <v>0.630564390054006</v>
       </c>
       <c r="C9" t="n">
-        <v>0.682018896940296</v>
+        <v>0.682018896940297</v>
       </c>
       <c r="D9" t="n">
-        <v>0.59483180202416</v>
+        <v>0.594831802024161</v>
       </c>
       <c r="E9" t="n">
-        <v>0.655976023165188</v>
+        <v>0.65597602316519</v>
       </c>
       <c r="F9" t="n">
-        <v>0.630564390054005</v>
+        <v>0.630564390054006</v>
       </c>
       <c r="G9" t="n">
-        <v>0.310905162143498</v>
+        <v>0.310905162143499</v>
       </c>
       <c r="H9" t="n">
         <v>0.501737112321151</v>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.992644332134456</v>
+        <v>0.993662990789622</v>
       </c>
     </row>
     <row r="10">
@@ -1011,28 +1011,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.651273032242981</v>
+        <v>0.648210257109439</v>
       </c>
       <c r="C10" t="n">
-        <v>0.703225805637433</v>
+        <v>0.704670473081782</v>
       </c>
       <c r="D10" t="n">
-        <v>0.588465941480315</v>
+        <v>0.584544350048525</v>
       </c>
       <c r="E10" t="n">
-        <v>0.656353425734274</v>
+        <v>0.65341028409551</v>
       </c>
       <c r="F10" t="n">
-        <v>0.651273032242981</v>
+        <v>0.648210257109439</v>
       </c>
       <c r="G10" t="n">
-        <v>0.31460310234753</v>
+        <v>0.312714475422796</v>
       </c>
       <c r="H10" t="n">
-        <v>0.512194996299063</v>
+        <v>0.514036263994266</v>
       </c>
       <c r="I10" t="n">
-        <v>0.992644332134456</v>
+        <v>0.993662990789622</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -1092,28 +1092,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.207645044667118</v>
+        <v>0.624982791919109</v>
       </c>
       <c r="D2" t="n">
-        <v>0.691612625923274</v>
+        <v>0.812541367629535</v>
       </c>
       <c r="E2" t="n">
-        <v>0.517158732924913</v>
+        <v>0.674445871153482</v>
       </c>
       <c r="F2" t="n">
-        <v>0.999994971764181</v>
+        <v>0.999995740440037</v>
       </c>
       <c r="G2" t="n">
-        <v>0.612582218182763</v>
+        <v>0.678695422554259</v>
       </c>
       <c r="H2" t="n">
-        <v>0.961099821491415</v>
+        <v>0.976286529237545</v>
       </c>
       <c r="I2" t="n">
-        <v>0.417736550638503</v>
+        <v>0.66205906750289</v>
       </c>
       <c r="J2" t="n">
-        <v>0.482128476843359</v>
+        <v>0.694519688486377</v>
       </c>
     </row>
     <row r="3">
@@ -1121,31 +1121,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.207645044667118</v>
+        <v>0.624982791919109</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.314233135158711</v>
+        <v>0.792970888885561</v>
       </c>
       <c r="E3" t="n">
-        <v>0.104544841272335</v>
+        <v>0.558277268643129</v>
       </c>
       <c r="F3" t="n">
-        <v>0.208296065586353</v>
+        <v>0.625365445792215</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0824902609722504</v>
+        <v>0.384458331098976</v>
       </c>
       <c r="H3" t="n">
-        <v>0.282295049512463</v>
+        <v>0.655186851112824</v>
       </c>
       <c r="I3" t="n">
-        <v>0.233738290093455</v>
+        <v>0.745003484921303</v>
       </c>
       <c r="J3" t="n">
-        <v>0.119717374591022</v>
+        <v>0.701956672862497</v>
       </c>
     </row>
     <row r="4">
@@ -1153,31 +1153,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.691612625923274</v>
+        <v>0.812541367629535</v>
       </c>
       <c r="C4" t="n">
-        <v>0.314233135158711</v>
+        <v>0.792970888885561</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.236063956766104</v>
+        <v>0.546427076438343</v>
       </c>
       <c r="F4" t="n">
-        <v>0.692070906165984</v>
+        <v>0.813261159800865</v>
       </c>
       <c r="G4" t="n">
-        <v>0.526419835106995</v>
+        <v>0.600226149448404</v>
       </c>
       <c r="H4" t="n">
-        <v>0.669870691879251</v>
+        <v>0.809493259653706</v>
       </c>
       <c r="I4" t="n">
-        <v>0.227941020003058</v>
+        <v>0.654477113342904</v>
       </c>
       <c r="J4" t="n">
-        <v>0.217008950645008</v>
+        <v>0.63239743655246</v>
       </c>
     </row>
     <row r="5">
@@ -1185,31 +1185,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.517158732924913</v>
+        <v>0.674445871153482</v>
       </c>
       <c r="C5" t="n">
-        <v>0.104544841272335</v>
+        <v>0.558277268643129</v>
       </c>
       <c r="D5" t="n">
-        <v>0.236063956766104</v>
+        <v>0.546427076438343</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.516693927446795</v>
+        <v>0.673352835175092</v>
       </c>
       <c r="G5" t="n">
-        <v>0.527621032795458</v>
+        <v>0.613085999706111</v>
       </c>
       <c r="H5" t="n">
-        <v>0.528466186142319</v>
+        <v>0.689546613902052</v>
       </c>
       <c r="I5" t="n">
-        <v>0.567686883562392</v>
+        <v>0.7238117869007</v>
       </c>
       <c r="J5" t="n">
-        <v>0.605429839810582</v>
+        <v>0.750325501119081</v>
       </c>
     </row>
     <row r="6">
@@ -1217,31 +1217,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.999994971764181</v>
+        <v>0.999995740440037</v>
       </c>
       <c r="C6" t="n">
-        <v>0.208296065586353</v>
+        <v>0.625365445792215</v>
       </c>
       <c r="D6" t="n">
-        <v>0.692070906165984</v>
+        <v>0.813261159800865</v>
       </c>
       <c r="E6" t="n">
-        <v>0.516693927446795</v>
+        <v>0.673352835175092</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.611305165590755</v>
+        <v>0.678008448509317</v>
       </c>
       <c r="H6" t="n">
-        <v>0.96105403686072</v>
+        <v>0.976195730067733</v>
       </c>
       <c r="I6" t="n">
-        <v>0.417643814822709</v>
+        <v>0.66181898788276</v>
       </c>
       <c r="J6" t="n">
-        <v>0.481965055052453</v>
+        <v>0.694168430752851</v>
       </c>
     </row>
     <row r="7">
@@ -1249,31 +1249,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.612582218182763</v>
+        <v>0.678695422554259</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0824902609722504</v>
+        <v>0.384458331098976</v>
       </c>
       <c r="D7" t="n">
-        <v>0.526419835106995</v>
+        <v>0.600226149448404</v>
       </c>
       <c r="E7" t="n">
-        <v>0.527621032795458</v>
+        <v>0.613085999706111</v>
       </c>
       <c r="F7" t="n">
-        <v>0.611305165590755</v>
+        <v>0.678008448509317</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.586261736020066</v>
+        <v>0.660564049921742</v>
       </c>
       <c r="I7" t="n">
-        <v>0.321335832581233</v>
+        <v>0.474913599758882</v>
       </c>
       <c r="J7" t="n">
-        <v>0.293831780603227</v>
+        <v>0.463113797610063</v>
       </c>
     </row>
     <row r="8">
@@ -1281,31 +1281,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.961099821491415</v>
+        <v>0.976286529237545</v>
       </c>
       <c r="C8" t="n">
-        <v>0.282295049512463</v>
+        <v>0.655186851112824</v>
       </c>
       <c r="D8" t="n">
-        <v>0.669870691879251</v>
+        <v>0.809493259653706</v>
       </c>
       <c r="E8" t="n">
-        <v>0.528466186142319</v>
+        <v>0.689546613902052</v>
       </c>
       <c r="F8" t="n">
-        <v>0.96105403686072</v>
+        <v>0.976195730067733</v>
       </c>
       <c r="G8" t="n">
-        <v>0.586261736020066</v>
+        <v>0.660564049921742</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.395639923399413</v>
+        <v>0.660690710661874</v>
       </c>
       <c r="J8" t="n">
-        <v>0.454725119316724</v>
+        <v>0.692032339219042</v>
       </c>
     </row>
     <row r="9">
@@ -1313,31 +1313,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.417736550638503</v>
+        <v>0.66205906750289</v>
       </c>
       <c r="C9" t="n">
-        <v>0.233738290093455</v>
+        <v>0.745003484921303</v>
       </c>
       <c r="D9" t="n">
-        <v>0.227941020003058</v>
+        <v>0.654477113342904</v>
       </c>
       <c r="E9" t="n">
-        <v>0.567686883562392</v>
+        <v>0.7238117869007</v>
       </c>
       <c r="F9" t="n">
-        <v>0.417643814822709</v>
+        <v>0.66181898788276</v>
       </c>
       <c r="G9" t="n">
-        <v>0.321335832581233</v>
+        <v>0.474913599758882</v>
       </c>
       <c r="H9" t="n">
-        <v>0.395639923399413</v>
+        <v>0.660690710661874</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.975026550794774</v>
+        <v>0.990631900855755</v>
       </c>
     </row>
     <row r="10">
@@ -1345,28 +1345,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.482128476843359</v>
+        <v>0.694519688486377</v>
       </c>
       <c r="C10" t="n">
-        <v>0.119717374591022</v>
+        <v>0.701956672862497</v>
       </c>
       <c r="D10" t="n">
-        <v>0.217008950645008</v>
+        <v>0.63239743655246</v>
       </c>
       <c r="E10" t="n">
-        <v>0.605429839810582</v>
+        <v>0.750325501119081</v>
       </c>
       <c r="F10" t="n">
-        <v>0.481965055052453</v>
+        <v>0.694168430752851</v>
       </c>
       <c r="G10" t="n">
-        <v>0.293831780603227</v>
+        <v>0.463113797610063</v>
       </c>
       <c r="H10" t="n">
-        <v>0.454725119316724</v>
+        <v>0.692032339219042</v>
       </c>
       <c r="I10" t="n">
-        <v>0.975026550794774</v>
+        <v>0.990631900855755</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -1426,28 +1426,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.990397954400231</v>
+        <v>0.988849715275415</v>
       </c>
       <c r="D2" t="n">
-        <v>0.917166170999469</v>
+        <v>0.92428788085608</v>
       </c>
       <c r="E2" t="n">
-        <v>0.879720966050802</v>
+        <v>0.920668781837191</v>
       </c>
       <c r="F2" t="n">
-        <v>0.999833173143633</v>
+        <v>0.99981934997977</v>
       </c>
       <c r="G2" t="n">
-        <v>0.71139133954549</v>
+        <v>0.755493329021262</v>
       </c>
       <c r="H2" t="n">
-        <v>0.967127186418626</v>
+        <v>0.970201317700409</v>
       </c>
       <c r="I2" t="n">
-        <v>0.484452289161165</v>
+        <v>0.580417197937779</v>
       </c>
       <c r="J2" t="n">
-        <v>0.554410771448858</v>
+        <v>0.59065893948856</v>
       </c>
     </row>
     <row r="3">
@@ -1455,31 +1455,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.990397954400231</v>
+        <v>0.988849715275415</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.88171046676749</v>
+        <v>0.90341180362917</v>
       </c>
       <c r="E3" t="n">
-        <v>0.911027159206104</v>
+        <v>0.946411503561118</v>
       </c>
       <c r="F3" t="n">
-        <v>0.989940241476772</v>
+        <v>0.989040738861475</v>
       </c>
       <c r="G3" t="n">
-        <v>0.704724986198702</v>
+        <v>0.753175524386079</v>
       </c>
       <c r="H3" t="n">
-        <v>0.948040442471345</v>
+        <v>0.950062395011655</v>
       </c>
       <c r="I3" t="n">
-        <v>0.459868981592563</v>
+        <v>0.579460900545654</v>
       </c>
       <c r="J3" t="n">
-        <v>0.521844670449959</v>
+        <v>0.576131659839682</v>
       </c>
     </row>
     <row r="4">
@@ -1487,31 +1487,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.917166170999469</v>
+        <v>0.92428788085608</v>
       </c>
       <c r="C4" t="n">
-        <v>0.88171046676749</v>
+        <v>0.90341180362917</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7123124747271</v>
+        <v>0.799027007932816</v>
       </c>
       <c r="F4" t="n">
-        <v>0.91772860808972</v>
+        <v>0.925271123314261</v>
       </c>
       <c r="G4" t="n">
-        <v>0.656765157959925</v>
+        <v>0.71643368093622</v>
       </c>
       <c r="H4" t="n">
-        <v>0.894066939396332</v>
+        <v>0.894089044330801</v>
       </c>
       <c r="I4" t="n">
-        <v>0.61129242183037</v>
+        <v>0.705439582136374</v>
       </c>
       <c r="J4" t="n">
-        <v>0.692477544905215</v>
+        <v>0.721861453194417</v>
       </c>
     </row>
     <row r="5">
@@ -1519,31 +1519,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.879720966050802</v>
+        <v>0.920668781837191</v>
       </c>
       <c r="C5" t="n">
-        <v>0.911027159206104</v>
+        <v>0.946411503561118</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7123124747271</v>
+        <v>0.799027007932816</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.877437938434078</v>
+        <v>0.919580953895728</v>
       </c>
       <c r="G5" t="n">
-        <v>0.611201727515635</v>
+        <v>0.682528171428574</v>
       </c>
       <c r="H5" t="n">
-        <v>0.851538082307824</v>
+        <v>0.905352400655372</v>
       </c>
       <c r="I5" t="n">
-        <v>0.267469294215084</v>
+        <v>0.435720306797409</v>
       </c>
       <c r="J5" t="n">
-        <v>0.30825363941735</v>
+        <v>0.420183551820716</v>
       </c>
     </row>
     <row r="6">
@@ -1551,31 +1551,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.999833173143633</v>
+        <v>0.99981934997977</v>
       </c>
       <c r="C6" t="n">
-        <v>0.989940241476772</v>
+        <v>0.989040738861475</v>
       </c>
       <c r="D6" t="n">
-        <v>0.91772860808972</v>
+        <v>0.925271123314261</v>
       </c>
       <c r="E6" t="n">
-        <v>0.877437938434078</v>
+        <v>0.919580953895728</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.71241838377386</v>
+        <v>0.756666106008344</v>
       </c>
       <c r="H6" t="n">
-        <v>0.966828596157581</v>
+        <v>0.969897220632698</v>
       </c>
       <c r="I6" t="n">
-        <v>0.490323493820187</v>
+        <v>0.586594741743409</v>
       </c>
       <c r="J6" t="n">
-        <v>0.559335596265989</v>
+        <v>0.595943801038257</v>
       </c>
     </row>
     <row r="7">
@@ -1583,31 +1583,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.71139133954549</v>
+        <v>0.755493329021262</v>
       </c>
       <c r="C7" t="n">
-        <v>0.704724986198702</v>
+        <v>0.753175524386079</v>
       </c>
       <c r="D7" t="n">
-        <v>0.656765157959925</v>
+        <v>0.71643368093622</v>
       </c>
       <c r="E7" t="n">
-        <v>0.611201727515635</v>
+        <v>0.682528171428574</v>
       </c>
       <c r="F7" t="n">
-        <v>0.71241838377386</v>
+        <v>0.756666106008344</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.69962317918028</v>
+        <v>0.74594274628566</v>
       </c>
       <c r="I7" t="n">
-        <v>0.595381548732653</v>
+        <v>0.665310826015147</v>
       </c>
       <c r="J7" t="n">
-        <v>0.600293045453397</v>
+        <v>0.648092150376006</v>
       </c>
     </row>
     <row r="8">
@@ -1615,31 +1615,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.967127186418626</v>
+        <v>0.970201317700409</v>
       </c>
       <c r="C8" t="n">
-        <v>0.948040442471345</v>
+        <v>0.950062395011655</v>
       </c>
       <c r="D8" t="n">
-        <v>0.894066939396332</v>
+        <v>0.894089044330801</v>
       </c>
       <c r="E8" t="n">
-        <v>0.851538082307824</v>
+        <v>0.905352400655372</v>
       </c>
       <c r="F8" t="n">
-        <v>0.966828596157581</v>
+        <v>0.969897220632698</v>
       </c>
       <c r="G8" t="n">
-        <v>0.69962317918028</v>
+        <v>0.74594274628566</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.483502281476617</v>
+        <v>0.569951978730284</v>
       </c>
       <c r="J8" t="n">
-        <v>0.561330395492104</v>
+        <v>0.584372674768833</v>
       </c>
     </row>
     <row r="9">
@@ -1647,31 +1647,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.484452289161165</v>
+        <v>0.580417197937779</v>
       </c>
       <c r="C9" t="n">
-        <v>0.459868981592563</v>
+        <v>0.579460900545654</v>
       </c>
       <c r="D9" t="n">
-        <v>0.61129242183037</v>
+        <v>0.705439582136374</v>
       </c>
       <c r="E9" t="n">
-        <v>0.267469294215084</v>
+        <v>0.435720306797409</v>
       </c>
       <c r="F9" t="n">
-        <v>0.490323493820187</v>
+        <v>0.586594741743409</v>
       </c>
       <c r="G9" t="n">
-        <v>0.595381548732653</v>
+        <v>0.665310826015147</v>
       </c>
       <c r="H9" t="n">
-        <v>0.483502281476617</v>
+        <v>0.569951978730284</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.987076681710489</v>
+        <v>0.991836735413815</v>
       </c>
     </row>
     <row r="10">
@@ -1679,28 +1679,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.554410771448858</v>
+        <v>0.59065893948856</v>
       </c>
       <c r="C10" t="n">
-        <v>0.521844670449959</v>
+        <v>0.576131659839682</v>
       </c>
       <c r="D10" t="n">
-        <v>0.692477544905215</v>
+        <v>0.721861453194417</v>
       </c>
       <c r="E10" t="n">
-        <v>0.30825363941735</v>
+        <v>0.420183551820716</v>
       </c>
       <c r="F10" t="n">
-        <v>0.559335596265989</v>
+        <v>0.595943801038257</v>
       </c>
       <c r="G10" t="n">
-        <v>0.600293045453397</v>
+        <v>0.648092150376006</v>
       </c>
       <c r="H10" t="n">
-        <v>0.561330395492104</v>
+        <v>0.584372674768833</v>
       </c>
       <c r="I10" t="n">
-        <v>0.987076681710489</v>
+        <v>0.991836735413815</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -1781,7 +1781,7 @@
         <v>0.514261224206667</v>
       </c>
       <c r="J2" t="n">
-        <v>0.579233131272517</v>
+        <v>0.570326150464124</v>
       </c>
     </row>
     <row r="3">
@@ -1795,13 +1795,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0941632034487094</v>
+        <v>-0.0941632034487108</v>
       </c>
       <c r="E3" t="n">
         <v>0.386028940693165</v>
       </c>
       <c r="F3" t="n">
-        <v>0.296924566397308</v>
+        <v>0.296924566397306</v>
       </c>
       <c r="G3" t="n">
         <v>-0.0403854416619807</v>
@@ -1810,10 +1810,10 @@
         <v>0.164199464565871</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.169199321014454</v>
+        <v>-0.169199321014453</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.145334975447322</v>
+        <v>-0.153406302783508</v>
       </c>
     </row>
     <row r="4">
@@ -1824,13 +1824,13 @@
         <v>0.758039087839085</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0941632034487094</v>
+        <v>-0.0941632034487108</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.526072308295134</v>
+        <v>0.526072308295133</v>
       </c>
       <c r="F4" t="n">
         <v>0.760973777791147</v>
@@ -1839,13 +1839,13 @@
         <v>0.85711714885472</v>
       </c>
       <c r="H4" t="n">
-        <v>0.742640382036383</v>
+        <v>0.742640382036382</v>
       </c>
       <c r="I4" t="n">
         <v>0.566115982487329</v>
       </c>
       <c r="J4" t="n">
-        <v>0.601938437462755</v>
+        <v>0.601549349112477</v>
       </c>
     </row>
     <row r="5">
@@ -1859,13 +1859,13 @@
         <v>0.386028940693165</v>
       </c>
       <c r="D5" t="n">
-        <v>0.526072308295134</v>
+        <v>0.526072308295133</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.831216591348442</v>
+        <v>0.831216591348443</v>
       </c>
       <c r="G5" t="n">
         <v>0.431224283273494</v>
@@ -1874,10 +1874,10 @@
         <v>0.753420337178228</v>
       </c>
       <c r="I5" t="n">
-        <v>0.215498569187857</v>
+        <v>0.215498569187856</v>
       </c>
       <c r="J5" t="n">
-        <v>0.278930326473224</v>
+        <v>0.270277596089024</v>
       </c>
     </row>
     <row r="6">
@@ -1888,13 +1888,13 @@
         <v>0.99997933133253</v>
       </c>
       <c r="C6" t="n">
-        <v>0.296924566397308</v>
+        <v>0.296924566397306</v>
       </c>
       <c r="D6" t="n">
         <v>0.760973777791147</v>
       </c>
       <c r="E6" t="n">
-        <v>0.831216591348442</v>
+        <v>0.831216591348443</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -1909,7 +1909,7 @@
         <v>0.517170806317209</v>
       </c>
       <c r="J6" t="n">
-        <v>0.581934188119687</v>
+        <v>0.573084681983609</v>
       </c>
     </row>
     <row r="7">
@@ -1938,10 +1938,10 @@
         <v>0.77171987903553</v>
       </c>
       <c r="I7" t="n">
-        <v>0.499449208242188</v>
+        <v>0.499449208242189</v>
       </c>
       <c r="J7" t="n">
-        <v>0.539721315251698</v>
+        <v>0.537942606977082</v>
       </c>
     </row>
     <row r="8">
@@ -1955,7 +1955,7 @@
         <v>0.164199464565871</v>
       </c>
       <c r="D8" t="n">
-        <v>0.742640382036383</v>
+        <v>0.742640382036382</v>
       </c>
       <c r="E8" t="n">
         <v>0.753420337178228</v>
@@ -1970,10 +1970,10 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.612352142759942</v>
+        <v>0.612352142759941</v>
       </c>
       <c r="J8" t="n">
-        <v>0.668856678820413</v>
+        <v>0.661711807893929</v>
       </c>
     </row>
     <row r="9">
@@ -1984,28 +1984,28 @@
         <v>0.514261224206667</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.169199321014454</v>
+        <v>-0.169199321014453</v>
       </c>
       <c r="D9" t="n">
         <v>0.566115982487329</v>
       </c>
       <c r="E9" t="n">
-        <v>0.215498569187857</v>
+        <v>0.215498569187856</v>
       </c>
       <c r="F9" t="n">
         <v>0.517170806317209</v>
       </c>
       <c r="G9" t="n">
-        <v>0.499449208242188</v>
+        <v>0.499449208242189</v>
       </c>
       <c r="H9" t="n">
-        <v>0.612352142759942</v>
+        <v>0.612352142759941</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.992654469152767</v>
+        <v>0.99345393386365</v>
       </c>
     </row>
     <row r="10">
@@ -2013,28 +2013,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.579233131272517</v>
+        <v>0.570326150464124</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.145334975447322</v>
+        <v>-0.153406302783508</v>
       </c>
       <c r="D10" t="n">
-        <v>0.601938437462755</v>
+        <v>0.601549349112477</v>
       </c>
       <c r="E10" t="n">
-        <v>0.278930326473224</v>
+        <v>0.270277596089024</v>
       </c>
       <c r="F10" t="n">
-        <v>0.581934188119687</v>
+        <v>0.573084681983609</v>
       </c>
       <c r="G10" t="n">
-        <v>0.539721315251698</v>
+        <v>0.537942606977082</v>
       </c>
       <c r="H10" t="n">
-        <v>0.668856678820413</v>
+        <v>0.661711807893929</v>
       </c>
       <c r="I10" t="n">
-        <v>0.992654469152767</v>
+        <v>0.99345393386365</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -2094,28 +2094,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.859270670066898</v>
+        <v>0.866065501819229</v>
       </c>
       <c r="D2" t="n">
-        <v>0.950409270859915</v>
+        <v>0.971896886159686</v>
       </c>
       <c r="E2" t="n">
-        <v>0.97171565586835</v>
+        <v>0.971630000137124</v>
       </c>
       <c r="F2" t="n">
-        <v>0.999768230023017</v>
+        <v>0.999733102220432</v>
       </c>
       <c r="G2" t="n">
-        <v>0.866650785002619</v>
+        <v>0.882370157880468</v>
       </c>
       <c r="H2" t="n">
-        <v>0.848373665266535</v>
+        <v>0.843266514550497</v>
       </c>
       <c r="I2" t="n">
-        <v>0.771468430640305</v>
+        <v>0.785374394640837</v>
       </c>
       <c r="J2" t="n">
-        <v>0.789711894194208</v>
+        <v>0.798349126563995</v>
       </c>
     </row>
     <row r="3">
@@ -2123,31 +2123,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.859270670066898</v>
+        <v>0.866065501819229</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.847799449861006</v>
+        <v>0.849579615954048</v>
       </c>
       <c r="E3" t="n">
-        <v>0.821889822453833</v>
+        <v>0.827014575358928</v>
       </c>
       <c r="F3" t="n">
-        <v>0.861885307851261</v>
+        <v>0.868618386526082</v>
       </c>
       <c r="G3" t="n">
-        <v>0.934567267724287</v>
+        <v>0.930689175719418</v>
       </c>
       <c r="H3" t="n">
-        <v>0.850922081351526</v>
+        <v>0.846308685621131</v>
       </c>
       <c r="I3" t="n">
-        <v>0.935289016959248</v>
+        <v>0.927747824969137</v>
       </c>
       <c r="J3" t="n">
-        <v>0.938063949234578</v>
+        <v>0.926941308004014</v>
       </c>
     </row>
     <row r="4">
@@ -2155,31 +2155,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.950409270859915</v>
+        <v>0.971896886159686</v>
       </c>
       <c r="C4" t="n">
-        <v>0.847799449861006</v>
+        <v>0.849579615954048</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.892457917770158</v>
+        <v>0.906223569308449</v>
       </c>
       <c r="F4" t="n">
-        <v>0.952324899794012</v>
+        <v>0.974230877914639</v>
       </c>
       <c r="G4" t="n">
-        <v>0.859677796515837</v>
+        <v>0.862424306415885</v>
       </c>
       <c r="H4" t="n">
-        <v>0.844483607465805</v>
+        <v>0.842262896878273</v>
       </c>
       <c r="I4" t="n">
-        <v>0.777293098827417</v>
+        <v>0.755113566242919</v>
       </c>
       <c r="J4" t="n">
-        <v>0.781793475483329</v>
+        <v>0.758459734337636</v>
       </c>
     </row>
     <row r="5">
@@ -2187,31 +2187,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.97171565586835</v>
+        <v>0.971630000137124</v>
       </c>
       <c r="C5" t="n">
-        <v>0.821889822453833</v>
+        <v>0.827014575358928</v>
       </c>
       <c r="D5" t="n">
-        <v>0.892457917770158</v>
+        <v>0.906223569308449</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.969094508356355</v>
+        <v>0.96822932211106</v>
       </c>
       <c r="G5" t="n">
-        <v>0.857331271753934</v>
+        <v>0.874274269256272</v>
       </c>
       <c r="H5" t="n">
-        <v>0.807584986852636</v>
+        <v>0.807904942123384</v>
       </c>
       <c r="I5" t="n">
-        <v>0.762170765313253</v>
+        <v>0.784506819050458</v>
       </c>
       <c r="J5" t="n">
-        <v>0.788119025242149</v>
+        <v>0.807152905889826</v>
       </c>
     </row>
     <row r="6">
@@ -2219,31 +2219,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.999768230023017</v>
+        <v>0.999733102220432</v>
       </c>
       <c r="C6" t="n">
-        <v>0.861885307851261</v>
+        <v>0.868618386526082</v>
       </c>
       <c r="D6" t="n">
-        <v>0.952324899794012</v>
+        <v>0.974230877914639</v>
       </c>
       <c r="E6" t="n">
-        <v>0.969094508356355</v>
+        <v>0.96822932211106</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.867729639418643</v>
+        <v>0.882720358198002</v>
       </c>
       <c r="H6" t="n">
-        <v>0.849033645574227</v>
+        <v>0.843523100408232</v>
       </c>
       <c r="I6" t="n">
-        <v>0.772410134916765</v>
+        <v>0.784965398491207</v>
       </c>
       <c r="J6" t="n">
-        <v>0.790114223457033</v>
+        <v>0.797124633926107</v>
       </c>
     </row>
     <row r="7">
@@ -2251,31 +2251,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.866650785002619</v>
+        <v>0.882370157880468</v>
       </c>
       <c r="C7" t="n">
-        <v>0.934567267724287</v>
+        <v>0.930689175719418</v>
       </c>
       <c r="D7" t="n">
-        <v>0.859677796515837</v>
+        <v>0.862424306415885</v>
       </c>
       <c r="E7" t="n">
-        <v>0.857331271753934</v>
+        <v>0.874274269256272</v>
       </c>
       <c r="F7" t="n">
-        <v>0.867729639418643</v>
+        <v>0.882720358198002</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.856620075349431</v>
+        <v>0.859625995920267</v>
       </c>
       <c r="I7" t="n">
-        <v>0.868018740787822</v>
+        <v>0.868603597025739</v>
       </c>
       <c r="J7" t="n">
-        <v>0.880859059541175</v>
+        <v>0.879323956705947</v>
       </c>
     </row>
     <row r="8">
@@ -2283,31 +2283,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.848373665266535</v>
+        <v>0.843266514550497</v>
       </c>
       <c r="C8" t="n">
-        <v>0.850922081351526</v>
+        <v>0.846308685621131</v>
       </c>
       <c r="D8" t="n">
-        <v>0.844483607465805</v>
+        <v>0.842262896878273</v>
       </c>
       <c r="E8" t="n">
-        <v>0.807584986852636</v>
+        <v>0.807904942123384</v>
       </c>
       <c r="F8" t="n">
-        <v>0.849033645574227</v>
+        <v>0.843523100408232</v>
       </c>
       <c r="G8" t="n">
-        <v>0.856620075349431</v>
+        <v>0.859625995920267</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.788020114186903</v>
+        <v>0.801412222685828</v>
       </c>
       <c r="J8" t="n">
-        <v>0.799903290478307</v>
+        <v>0.807467578075638</v>
       </c>
     </row>
     <row r="9">
@@ -2315,31 +2315,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.771468430640305</v>
+        <v>0.785374394640837</v>
       </c>
       <c r="C9" t="n">
-        <v>0.935289016959248</v>
+        <v>0.927747824969137</v>
       </c>
       <c r="D9" t="n">
-        <v>0.777293098827417</v>
+        <v>0.755113566242919</v>
       </c>
       <c r="E9" t="n">
-        <v>0.762170765313253</v>
+        <v>0.784506819050458</v>
       </c>
       <c r="F9" t="n">
-        <v>0.772410134916765</v>
+        <v>0.784965398491207</v>
       </c>
       <c r="G9" t="n">
-        <v>0.868018740787822</v>
+        <v>0.868603597025739</v>
       </c>
       <c r="H9" t="n">
-        <v>0.788020114186903</v>
+        <v>0.801412222685828</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.997370610780788</v>
+        <v>0.997212536423374</v>
       </c>
     </row>
     <row r="10">
@@ -2347,28 +2347,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.789711894194208</v>
+        <v>0.798349126563995</v>
       </c>
       <c r="C10" t="n">
-        <v>0.938063949234578</v>
+        <v>0.926941308004014</v>
       </c>
       <c r="D10" t="n">
-        <v>0.781793475483329</v>
+        <v>0.758459734337636</v>
       </c>
       <c r="E10" t="n">
-        <v>0.788119025242149</v>
+        <v>0.807152905889826</v>
       </c>
       <c r="F10" t="n">
-        <v>0.790114223457033</v>
+        <v>0.797124633926107</v>
       </c>
       <c r="G10" t="n">
-        <v>0.880859059541175</v>
+        <v>0.879323956705947</v>
       </c>
       <c r="H10" t="n">
-        <v>0.799903290478307</v>
+        <v>0.807467578075638</v>
       </c>
       <c r="I10" t="n">
-        <v>0.997370610780788</v>
+        <v>0.997212536423374</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -2428,28 +2428,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.956406023194335</v>
+        <v>0.953991250814815</v>
       </c>
       <c r="D2" t="n">
-        <v>0.975571140762151</v>
+        <v>0.972171888079616</v>
       </c>
       <c r="E2" t="n">
-        <v>0.992046575491689</v>
+        <v>0.99208096882837</v>
       </c>
       <c r="F2" t="n">
-        <v>0.999885158567627</v>
+        <v>0.999880576262506</v>
       </c>
       <c r="G2" t="n">
-        <v>0.938932148070597</v>
+        <v>0.934237033668305</v>
       </c>
       <c r="H2" t="n">
-        <v>0.992666901842216</v>
+        <v>0.99319239219303</v>
       </c>
       <c r="I2" t="n">
-        <v>0.825319180533896</v>
+        <v>0.811983413845089</v>
       </c>
       <c r="J2" t="n">
-        <v>0.845702253999694</v>
+        <v>0.836822999926332</v>
       </c>
     </row>
     <row r="3">
@@ -2457,31 +2457,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.956406023194335</v>
+        <v>0.953991250814815</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.917601350350372</v>
+        <v>0.909102559598899</v>
       </c>
       <c r="E3" t="n">
-        <v>0.943870038941794</v>
+        <v>0.942317019264768</v>
       </c>
       <c r="F3" t="n">
-        <v>0.957617767880566</v>
+        <v>0.955177619059603</v>
       </c>
       <c r="G3" t="n">
-        <v>0.886912921807063</v>
+        <v>0.87818752017642</v>
       </c>
       <c r="H3" t="n">
-        <v>0.94588110339058</v>
+        <v>0.944281632204618</v>
       </c>
       <c r="I3" t="n">
-        <v>0.720225112400211</v>
+        <v>0.701196408859102</v>
       </c>
       <c r="J3" t="n">
-        <v>0.741557500539155</v>
+        <v>0.730724886310794</v>
       </c>
     </row>
     <row r="4">
@@ -2489,31 +2489,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.975571140762151</v>
+        <v>0.972171888079616</v>
       </c>
       <c r="C4" t="n">
-        <v>0.917601350350372</v>
+        <v>0.909102559598899</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.977818408146053</v>
+        <v>0.974811173277785</v>
       </c>
       <c r="F4" t="n">
-        <v>0.97323287454938</v>
+        <v>0.969616084107063</v>
       </c>
       <c r="G4" t="n">
-        <v>0.954237247516359</v>
+        <v>0.954403423394322</v>
       </c>
       <c r="H4" t="n">
-        <v>0.959445882403236</v>
+        <v>0.957302342815812</v>
       </c>
       <c r="I4" t="n">
-        <v>0.843934896967047</v>
+        <v>0.832072534163746</v>
       </c>
       <c r="J4" t="n">
-        <v>0.860465725428556</v>
+        <v>0.850308672688181</v>
       </c>
     </row>
     <row r="5">
@@ -2521,31 +2521,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.992046575491689</v>
+        <v>0.99208096882837</v>
       </c>
       <c r="C5" t="n">
-        <v>0.943870038941794</v>
+        <v>0.942317019264768</v>
       </c>
       <c r="D5" t="n">
-        <v>0.977818408146053</v>
+        <v>0.974811173277785</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.991590147297917</v>
+        <v>0.991679172078859</v>
       </c>
       <c r="G5" t="n">
-        <v>0.958214963997381</v>
+        <v>0.954568365342069</v>
       </c>
       <c r="H5" t="n">
-        <v>0.989121924654478</v>
+        <v>0.989228181965176</v>
       </c>
       <c r="I5" t="n">
-        <v>0.827788022318663</v>
+        <v>0.812466550550949</v>
       </c>
       <c r="J5" t="n">
-        <v>0.845848742403135</v>
+        <v>0.834691765822692</v>
       </c>
     </row>
     <row r="6">
@@ -2553,31 +2553,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.999885158567627</v>
+        <v>0.999880576262506</v>
       </c>
       <c r="C6" t="n">
-        <v>0.957617767880566</v>
+        <v>0.955177619059603</v>
       </c>
       <c r="D6" t="n">
-        <v>0.97323287454938</v>
+        <v>0.969616084107063</v>
       </c>
       <c r="E6" t="n">
-        <v>0.991590147297917</v>
+        <v>0.991679172078859</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.936400243501571</v>
+        <v>0.93137819498886</v>
       </c>
       <c r="H6" t="n">
-        <v>0.99286101783135</v>
+        <v>0.993340634536752</v>
       </c>
       <c r="I6" t="n">
-        <v>0.822173278185245</v>
+        <v>0.808666505339911</v>
       </c>
       <c r="J6" t="n">
-        <v>0.842697930813518</v>
+        <v>0.833866491539116</v>
       </c>
     </row>
     <row r="7">
@@ -2585,31 +2585,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.938932148070597</v>
+        <v>0.934237033668305</v>
       </c>
       <c r="C7" t="n">
-        <v>0.886912921807063</v>
+        <v>0.87818752017642</v>
       </c>
       <c r="D7" t="n">
-        <v>0.954237247516359</v>
+        <v>0.954403423394322</v>
       </c>
       <c r="E7" t="n">
-        <v>0.958214963997381</v>
+        <v>0.954568365342069</v>
       </c>
       <c r="F7" t="n">
-        <v>0.936400243501571</v>
+        <v>0.93137819498886</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.93234320431193</v>
+        <v>0.924262195143476</v>
       </c>
       <c r="I7" t="n">
-        <v>0.755252960379712</v>
+        <v>0.738627635908049</v>
       </c>
       <c r="J7" t="n">
-        <v>0.769911072448862</v>
+        <v>0.755278254638953</v>
       </c>
     </row>
     <row r="8">
@@ -2617,31 +2617,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.992666901842216</v>
+        <v>0.99319239219303</v>
       </c>
       <c r="C8" t="n">
-        <v>0.94588110339058</v>
+        <v>0.944281632204618</v>
       </c>
       <c r="D8" t="n">
-        <v>0.959445882403236</v>
+        <v>0.957302342815812</v>
       </c>
       <c r="E8" t="n">
-        <v>0.989121924654478</v>
+        <v>0.989228181965176</v>
       </c>
       <c r="F8" t="n">
-        <v>0.99286101783135</v>
+        <v>0.993340634536752</v>
       </c>
       <c r="G8" t="n">
-        <v>0.93234320431193</v>
+        <v>0.924262195143476</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.833844971862208</v>
+        <v>0.825470762091539</v>
       </c>
       <c r="J8" t="n">
-        <v>0.85126082948169</v>
+        <v>0.848223126835623</v>
       </c>
     </row>
     <row r="9">
@@ -2649,31 +2649,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.825319180533896</v>
+        <v>0.811983413845089</v>
       </c>
       <c r="C9" t="n">
-        <v>0.720225112400211</v>
+        <v>0.701196408859102</v>
       </c>
       <c r="D9" t="n">
-        <v>0.843934896967047</v>
+        <v>0.832072534163746</v>
       </c>
       <c r="E9" t="n">
-        <v>0.827788022318663</v>
+        <v>0.812466550550949</v>
       </c>
       <c r="F9" t="n">
-        <v>0.822173278185245</v>
+        <v>0.808666505339911</v>
       </c>
       <c r="G9" t="n">
-        <v>0.755252960379712</v>
+        <v>0.738627635908049</v>
       </c>
       <c r="H9" t="n">
-        <v>0.833844971862208</v>
+        <v>0.825470762091539</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.997484645526175</v>
+        <v>0.99755184600067</v>
       </c>
     </row>
     <row r="10">
@@ -2681,28 +2681,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.845702253999694</v>
+        <v>0.836822999926332</v>
       </c>
       <c r="C10" t="n">
-        <v>0.741557500539155</v>
+        <v>0.730724886310794</v>
       </c>
       <c r="D10" t="n">
-        <v>0.860465725428556</v>
+        <v>0.850308672688181</v>
       </c>
       <c r="E10" t="n">
-        <v>0.845848742403135</v>
+        <v>0.834691765822692</v>
       </c>
       <c r="F10" t="n">
-        <v>0.842697930813518</v>
+        <v>0.833866491539116</v>
       </c>
       <c r="G10" t="n">
-        <v>0.769911072448862</v>
+        <v>0.755278254638953</v>
       </c>
       <c r="H10" t="n">
-        <v>0.85126082948169</v>
+        <v>0.848223126835623</v>
       </c>
       <c r="I10" t="n">
-        <v>0.997484645526175</v>
+        <v>0.99755184600067</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -2762,28 +2762,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.996692655132861</v>
+        <v>0.996596154457917</v>
       </c>
       <c r="D2" t="n">
-        <v>0.875544880648104</v>
+        <v>0.942065538187833</v>
       </c>
       <c r="E2" t="n">
-        <v>0.999463284627583</v>
+        <v>0.999566782401067</v>
       </c>
       <c r="F2" t="n">
-        <v>0.995433694346232</v>
+        <v>0.995218630002075</v>
       </c>
       <c r="G2" t="n">
-        <v>0.970302046187234</v>
+        <v>0.967683142535246</v>
       </c>
       <c r="H2" t="n">
-        <v>0.88962863114755</v>
+        <v>0.859880222674014</v>
       </c>
       <c r="I2" t="n">
-        <v>0.808862502041319</v>
+        <v>0.767563508926053</v>
       </c>
       <c r="J2" t="n">
-        <v>0.823917614162741</v>
+        <v>0.788467425024513</v>
       </c>
     </row>
     <row r="3">
@@ -2791,31 +2791,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.996692655132861</v>
+        <v>0.996596154457917</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.87797193113064</v>
+        <v>0.94401803207309</v>
       </c>
       <c r="E3" t="n">
-        <v>0.997350213182772</v>
+        <v>0.997620368725479</v>
       </c>
       <c r="F3" t="n">
-        <v>0.990850045188776</v>
+        <v>0.991359254634068</v>
       </c>
       <c r="G3" t="n">
-        <v>0.961694158366694</v>
+        <v>0.963284973889641</v>
       </c>
       <c r="H3" t="n">
-        <v>0.879873615065295</v>
+        <v>0.838677776008677</v>
       </c>
       <c r="I3" t="n">
-        <v>0.806382749912665</v>
+        <v>0.772825655750658</v>
       </c>
       <c r="J3" t="n">
-        <v>0.821763891036364</v>
+        <v>0.793158472027154</v>
       </c>
     </row>
     <row r="4">
@@ -2823,31 +2823,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.875544880648104</v>
+        <v>0.942065538187833</v>
       </c>
       <c r="C4" t="n">
-        <v>0.87797193113064</v>
+        <v>0.94401803207309</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.881528914329856</v>
+        <v>0.945000148969151</v>
       </c>
       <c r="F4" t="n">
-        <v>0.859207128636046</v>
+        <v>0.943522942754811</v>
       </c>
       <c r="G4" t="n">
-        <v>0.852349631070444</v>
+        <v>0.968164050154087</v>
       </c>
       <c r="H4" t="n">
-        <v>0.76224346019015</v>
+        <v>0.739052425899765</v>
       </c>
       <c r="I4" t="n">
-        <v>0.592957629017263</v>
+        <v>0.617174489250128</v>
       </c>
       <c r="J4" t="n">
-        <v>0.604783830366706</v>
+        <v>0.632717294575179</v>
       </c>
     </row>
     <row r="5">
@@ -2855,31 +2855,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.999463284627583</v>
+        <v>0.999566782401067</v>
       </c>
       <c r="C5" t="n">
-        <v>0.997350213182772</v>
+        <v>0.997620368725479</v>
       </c>
       <c r="D5" t="n">
-        <v>0.881528914329856</v>
+        <v>0.945000148969151</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.994926839247362</v>
+        <v>0.995041869956887</v>
       </c>
       <c r="G5" t="n">
-        <v>0.972036073564512</v>
+        <v>0.969529933415834</v>
       </c>
       <c r="H5" t="n">
-        <v>0.884398717733394</v>
+        <v>0.856142894839559</v>
       </c>
       <c r="I5" t="n">
-        <v>0.804677370438645</v>
+        <v>0.763833497558117</v>
       </c>
       <c r="J5" t="n">
-        <v>0.818946132365113</v>
+        <v>0.784383419288349</v>
       </c>
     </row>
     <row r="6">
@@ -2887,31 +2887,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.995433694346232</v>
+        <v>0.995218630002075</v>
       </c>
       <c r="C6" t="n">
-        <v>0.990850045188776</v>
+        <v>0.991359254634068</v>
       </c>
       <c r="D6" t="n">
-        <v>0.859207128636046</v>
+        <v>0.943522942754811</v>
       </c>
       <c r="E6" t="n">
-        <v>0.994926839247362</v>
+        <v>0.995041869956887</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.979890133076578</v>
+        <v>0.978214719416028</v>
       </c>
       <c r="H6" t="n">
-        <v>0.876185925478506</v>
+        <v>0.841067790818497</v>
       </c>
       <c r="I6" t="n">
-        <v>0.801599496930999</v>
+        <v>0.756984751025298</v>
       </c>
       <c r="J6" t="n">
-        <v>0.814462019649287</v>
+        <v>0.776638619066412</v>
       </c>
     </row>
     <row r="7">
@@ -2919,31 +2919,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.970302046187234</v>
+        <v>0.967683142535246</v>
       </c>
       <c r="C7" t="n">
-        <v>0.961694158366694</v>
+        <v>0.963284973889641</v>
       </c>
       <c r="D7" t="n">
-        <v>0.852349631070444</v>
+        <v>0.968164050154087</v>
       </c>
       <c r="E7" t="n">
-        <v>0.972036073564512</v>
+        <v>0.969529933415834</v>
       </c>
       <c r="F7" t="n">
-        <v>0.979890133076578</v>
+        <v>0.978214719416028</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.82410340837164</v>
+        <v>0.781354753295442</v>
       </c>
       <c r="I7" t="n">
-        <v>0.721170861837909</v>
+        <v>0.665521537962339</v>
       </c>
       <c r="J7" t="n">
-        <v>0.727994335681354</v>
+        <v>0.681113325295988</v>
       </c>
     </row>
     <row r="8">
@@ -2951,31 +2951,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.88962863114755</v>
+        <v>0.859880222674014</v>
       </c>
       <c r="C8" t="n">
-        <v>0.879873615065295</v>
+        <v>0.838677776008677</v>
       </c>
       <c r="D8" t="n">
-        <v>0.76224346019015</v>
+        <v>0.739052425899765</v>
       </c>
       <c r="E8" t="n">
-        <v>0.884398717733394</v>
+        <v>0.856142894839559</v>
       </c>
       <c r="F8" t="n">
-        <v>0.876185925478506</v>
+        <v>0.841067790818497</v>
       </c>
       <c r="G8" t="n">
-        <v>0.82410340837164</v>
+        <v>0.781354753295442</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.763114367516357</v>
+        <v>0.701424023944668</v>
       </c>
       <c r="J8" t="n">
-        <v>0.776373914277474</v>
+        <v>0.717199884726772</v>
       </c>
     </row>
     <row r="9">
@@ -2983,31 +2983,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.808862502041319</v>
+        <v>0.767563508926053</v>
       </c>
       <c r="C9" t="n">
-        <v>0.806382749912665</v>
+        <v>0.772825655750658</v>
       </c>
       <c r="D9" t="n">
-        <v>0.592957629017263</v>
+        <v>0.617174489250128</v>
       </c>
       <c r="E9" t="n">
-        <v>0.804677370438645</v>
+        <v>0.763833497558117</v>
       </c>
       <c r="F9" t="n">
-        <v>0.801599496930999</v>
+        <v>0.756984751025298</v>
       </c>
       <c r="G9" t="n">
-        <v>0.721170861837909</v>
+        <v>0.665521537962339</v>
       </c>
       <c r="H9" t="n">
-        <v>0.763114367516357</v>
+        <v>0.701424023944668</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.996465357515158</v>
+        <v>0.997290597010274</v>
       </c>
     </row>
     <row r="10">
@@ -3015,28 +3015,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.823917614162741</v>
+        <v>0.788467425024513</v>
       </c>
       <c r="C10" t="n">
-        <v>0.821763891036364</v>
+        <v>0.793158472027154</v>
       </c>
       <c r="D10" t="n">
-        <v>0.604783830366706</v>
+        <v>0.632717294575179</v>
       </c>
       <c r="E10" t="n">
-        <v>0.818946132365113</v>
+        <v>0.784383419288349</v>
       </c>
       <c r="F10" t="n">
-        <v>0.814462019649287</v>
+        <v>0.776638619066412</v>
       </c>
       <c r="G10" t="n">
-        <v>0.727994335681354</v>
+        <v>0.681113325295988</v>
       </c>
       <c r="H10" t="n">
-        <v>0.776373914277474</v>
+        <v>0.717199884726772</v>
       </c>
       <c r="I10" t="n">
-        <v>0.996465357515158</v>
+        <v>0.997290597010274</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -3096,28 +3096,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.258182325502382</v>
+        <v>0.314964784834138</v>
       </c>
       <c r="D2" t="n">
-        <v>0.803381866754163</v>
+        <v>0.828102095516334</v>
       </c>
       <c r="E2" t="n">
-        <v>0.679435322960478</v>
+        <v>0.725815878915089</v>
       </c>
       <c r="F2" t="n">
-        <v>0.999421845261986</v>
+        <v>0.999456898684594</v>
       </c>
       <c r="G2" t="n">
-        <v>0.867551817965724</v>
+        <v>0.883697199222043</v>
       </c>
       <c r="H2" t="n">
-        <v>0.673844135857375</v>
+        <v>0.685378700081603</v>
       </c>
       <c r="I2" t="n">
-        <v>0.749580214814104</v>
+        <v>0.769820418174535</v>
       </c>
       <c r="J2" t="n">
-        <v>0.753085072663563</v>
+        <v>0.772768607623949</v>
       </c>
     </row>
     <row r="3">
@@ -3125,31 +3125,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.258182325502382</v>
+        <v>0.314964784834138</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.711576514939942</v>
+        <v>0.735589364418794</v>
       </c>
       <c r="E3" t="n">
-        <v>0.814647407208159</v>
+        <v>0.815907066718201</v>
       </c>
       <c r="F3" t="n">
-        <v>0.254527367307144</v>
+        <v>0.31080160092545</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.0541001448423336</v>
+        <v>0.0230713732143384</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.00161132475832166</v>
+        <v>0.0544546608194771</v>
       </c>
       <c r="I3" t="n">
-        <v>0.19046177679894</v>
+        <v>0.278453883666894</v>
       </c>
       <c r="J3" t="n">
-        <v>0.217824549384171</v>
+        <v>0.303440684847387</v>
       </c>
     </row>
     <row r="4">
@@ -3157,31 +3157,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.803381866754163</v>
+        <v>0.828102095516334</v>
       </c>
       <c r="C4" t="n">
-        <v>0.711576514939942</v>
+        <v>0.735589364418794</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.920221748156331</v>
+        <v>0.940279807269599</v>
       </c>
       <c r="F4" t="n">
-        <v>0.799522910542862</v>
+        <v>0.823856039024114</v>
       </c>
       <c r="G4" t="n">
-        <v>0.588212394572829</v>
+        <v>0.629597704761201</v>
       </c>
       <c r="H4" t="n">
-        <v>0.480577861964167</v>
+        <v>0.500722361459386</v>
       </c>
       <c r="I4" t="n">
-        <v>0.591394430128304</v>
+        <v>0.648659671098751</v>
       </c>
       <c r="J4" t="n">
-        <v>0.613521528327613</v>
+        <v>0.663812266964604</v>
       </c>
     </row>
     <row r="5">
@@ -3189,31 +3189,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.679435322960478</v>
+        <v>0.725815878915089</v>
       </c>
       <c r="C5" t="n">
-        <v>0.814647407208159</v>
+        <v>0.815907066718201</v>
       </c>
       <c r="D5" t="n">
-        <v>0.920221748156331</v>
+        <v>0.940279807269599</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.674974528389503</v>
+        <v>0.721075905583754</v>
       </c>
       <c r="G5" t="n">
-        <v>0.370793744211567</v>
+        <v>0.454011754557395</v>
       </c>
       <c r="H5" t="n">
-        <v>0.242648834203117</v>
+        <v>0.302341942580948</v>
       </c>
       <c r="I5" t="n">
-        <v>0.608435143570733</v>
+        <v>0.680817734293574</v>
       </c>
       <c r="J5" t="n">
-        <v>0.63446936225326</v>
+        <v>0.702972746258232</v>
       </c>
     </row>
     <row r="6">
@@ -3221,31 +3221,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.999421845261986</v>
+        <v>0.999456898684594</v>
       </c>
       <c r="C6" t="n">
-        <v>0.254527367307144</v>
+        <v>0.31080160092545</v>
       </c>
       <c r="D6" t="n">
-        <v>0.799522910542862</v>
+        <v>0.823856039024114</v>
       </c>
       <c r="E6" t="n">
-        <v>0.674974528389503</v>
+        <v>0.721075905583754</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.864329017580833</v>
+        <v>0.880208439880582</v>
       </c>
       <c r="H6" t="n">
-        <v>0.67965803996275</v>
+        <v>0.690990991549009</v>
       </c>
       <c r="I6" t="n">
-        <v>0.740139519158549</v>
+        <v>0.760475459395085</v>
       </c>
       <c r="J6" t="n">
-        <v>0.742976262537293</v>
+        <v>0.762882858960397</v>
       </c>
     </row>
     <row r="7">
@@ -3253,31 +3253,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.867551817965724</v>
+        <v>0.883697199222043</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0541001448423336</v>
+        <v>0.0230713732143384</v>
       </c>
       <c r="D7" t="n">
-        <v>0.588212394572829</v>
+        <v>0.629597704761201</v>
       </c>
       <c r="E7" t="n">
-        <v>0.370793744211567</v>
+        <v>0.454011754557395</v>
       </c>
       <c r="F7" t="n">
-        <v>0.864329017580833</v>
+        <v>0.880208439880582</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.656559914549081</v>
+        <v>0.665953082155386</v>
       </c>
       <c r="I7" t="n">
-        <v>0.657665267024458</v>
+        <v>0.660195274453372</v>
       </c>
       <c r="J7" t="n">
-        <v>0.662312962108652</v>
+        <v>0.660057520776772</v>
       </c>
     </row>
     <row r="8">
@@ -3285,31 +3285,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.673844135857375</v>
+        <v>0.685378700081603</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.00161132475832166</v>
+        <v>0.0544546608194771</v>
       </c>
       <c r="D8" t="n">
-        <v>0.480577861964167</v>
+        <v>0.500722361459386</v>
       </c>
       <c r="E8" t="n">
-        <v>0.242648834203117</v>
+        <v>0.302341942580948</v>
       </c>
       <c r="F8" t="n">
-        <v>0.67965803996275</v>
+        <v>0.690990991549009</v>
       </c>
       <c r="G8" t="n">
-        <v>0.656559914549081</v>
+        <v>0.665953082155386</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.319498493038542</v>
+        <v>0.32552777873317</v>
       </c>
       <c r="J8" t="n">
-        <v>0.309388723966844</v>
+        <v>0.318273776494613</v>
       </c>
     </row>
     <row r="9">
@@ -3317,31 +3317,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.749580214814104</v>
+        <v>0.769820418174535</v>
       </c>
       <c r="C9" t="n">
-        <v>0.19046177679894</v>
+        <v>0.278453883666894</v>
       </c>
       <c r="D9" t="n">
-        <v>0.591394430128304</v>
+        <v>0.648659671098751</v>
       </c>
       <c r="E9" t="n">
-        <v>0.608435143570733</v>
+        <v>0.680817734293574</v>
       </c>
       <c r="F9" t="n">
-        <v>0.740139519158549</v>
+        <v>0.760475459395085</v>
       </c>
       <c r="G9" t="n">
-        <v>0.657665267024458</v>
+        <v>0.660195274453372</v>
       </c>
       <c r="H9" t="n">
-        <v>0.319498493038542</v>
+        <v>0.32552777873317</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.997036027248689</v>
+        <v>0.997772879693637</v>
       </c>
     </row>
     <row r="10">
@@ -3349,28 +3349,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.753085072663563</v>
+        <v>0.772768607623949</v>
       </c>
       <c r="C10" t="n">
-        <v>0.217824549384171</v>
+        <v>0.303440684847387</v>
       </c>
       <c r="D10" t="n">
-        <v>0.613521528327613</v>
+        <v>0.663812266964604</v>
       </c>
       <c r="E10" t="n">
-        <v>0.63446936225326</v>
+        <v>0.702972746258232</v>
       </c>
       <c r="F10" t="n">
-        <v>0.742976262537293</v>
+        <v>0.762882858960397</v>
       </c>
       <c r="G10" t="n">
-        <v>0.662312962108652</v>
+        <v>0.660057520776772</v>
       </c>
       <c r="H10" t="n">
-        <v>0.309388723966844</v>
+        <v>0.318273776494613</v>
       </c>
       <c r="I10" t="n">
-        <v>0.997036027248689</v>
+        <v>0.997772879693637</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -3430,28 +3430,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.997392089568306</v>
+        <v>0.99735142231637</v>
       </c>
       <c r="D2" t="n">
-        <v>0.971547651052648</v>
+        <v>0.991787192562141</v>
       </c>
       <c r="E2" t="n">
-        <v>0.985568748800276</v>
+        <v>0.993183924941267</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.953775371221614</v>
+        <v>0.960103951857091</v>
       </c>
       <c r="H2" t="n">
-        <v>0.996642260759863</v>
+        <v>0.996904353072825</v>
       </c>
       <c r="I2" t="n">
-        <v>0.818375625288924</v>
+        <v>0.876244855766799</v>
       </c>
       <c r="J2" t="n">
-        <v>0.870977583088279</v>
+        <v>0.904892167412491</v>
       </c>
     </row>
     <row r="3">
@@ -3459,31 +3459,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.997392089568306</v>
+        <v>0.99735142231637</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.964812956135928</v>
+        <v>0.98430397442474</v>
       </c>
       <c r="E3" t="n">
-        <v>0.976497623704649</v>
+        <v>0.985728390570978</v>
       </c>
       <c r="F3" t="n">
-        <v>0.997392089568306</v>
+        <v>0.99735142231637</v>
       </c>
       <c r="G3" t="n">
-        <v>0.947361100118237</v>
+        <v>0.953455549814823</v>
       </c>
       <c r="H3" t="n">
-        <v>0.994821228519139</v>
+        <v>0.994941588616776</v>
       </c>
       <c r="I3" t="n">
-        <v>0.820224846236063</v>
+        <v>0.885407614209791</v>
       </c>
       <c r="J3" t="n">
-        <v>0.87393226914879</v>
+        <v>0.912659364609705</v>
       </c>
     </row>
     <row r="4">
@@ -3491,31 +3491,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.971547651052648</v>
+        <v>0.991787192562141</v>
       </c>
       <c r="C4" t="n">
-        <v>0.964812956135928</v>
+        <v>0.98430397442474</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.974164629669258</v>
+        <v>0.994919827998263</v>
       </c>
       <c r="F4" t="n">
-        <v>0.971547651052648</v>
+        <v>0.991787192562141</v>
       </c>
       <c r="G4" t="n">
-        <v>0.954930219606529</v>
+        <v>0.968285181102487</v>
       </c>
       <c r="H4" t="n">
-        <v>0.967510194691389</v>
+        <v>0.987159279821831</v>
       </c>
       <c r="I4" t="n">
-        <v>0.846858464097846</v>
+        <v>0.860687389076927</v>
       </c>
       <c r="J4" t="n">
-        <v>0.886670169863167</v>
+        <v>0.885685258450788</v>
       </c>
     </row>
     <row r="5">
@@ -3523,31 +3523,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.985568748800276</v>
+        <v>0.993183924941267</v>
       </c>
       <c r="C5" t="n">
-        <v>0.976497623704649</v>
+        <v>0.985728390570978</v>
       </c>
       <c r="D5" t="n">
-        <v>0.974164629669258</v>
+        <v>0.994919827998263</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.985568748800276</v>
+        <v>0.993183924941267</v>
       </c>
       <c r="G5" t="n">
-        <v>0.968093888382657</v>
+        <v>0.96989753878381</v>
       </c>
       <c r="H5" t="n">
-        <v>0.980500874128801</v>
+        <v>0.989473391335375</v>
       </c>
       <c r="I5" t="n">
-        <v>0.802651934729086</v>
+        <v>0.838878843379912</v>
       </c>
       <c r="J5" t="n">
-        <v>0.84453909044488</v>
+        <v>0.867518069945954</v>
       </c>
     </row>
     <row r="6">
@@ -3558,28 +3558,28 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.997392089568306</v>
+        <v>0.99735142231637</v>
       </c>
       <c r="D6" t="n">
-        <v>0.971547651052648</v>
+        <v>0.991787192562141</v>
       </c>
       <c r="E6" t="n">
-        <v>0.985568748800276</v>
+        <v>0.993183924941267</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.953775371221614</v>
+        <v>0.960103951857091</v>
       </c>
       <c r="H6" t="n">
-        <v>0.996642260759863</v>
+        <v>0.996904353072825</v>
       </c>
       <c r="I6" t="n">
-        <v>0.818375625288924</v>
+        <v>0.876244855766799</v>
       </c>
       <c r="J6" t="n">
-        <v>0.870977583088279</v>
+        <v>0.904892167412491</v>
       </c>
     </row>
     <row r="7">
@@ -3587,31 +3587,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.953775371221614</v>
+        <v>0.960103951857091</v>
       </c>
       <c r="C7" t="n">
-        <v>0.947361100118237</v>
+        <v>0.953455549814823</v>
       </c>
       <c r="D7" t="n">
-        <v>0.954930219606529</v>
+        <v>0.968285181102487</v>
       </c>
       <c r="E7" t="n">
-        <v>0.968093888382657</v>
+        <v>0.96989753878381</v>
       </c>
       <c r="F7" t="n">
-        <v>0.953775371221614</v>
+        <v>0.960103951857091</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.949348722284016</v>
+        <v>0.956710660935478</v>
       </c>
       <c r="I7" t="n">
-        <v>0.775872758155764</v>
+        <v>0.813843976608873</v>
       </c>
       <c r="J7" t="n">
-        <v>0.823159918238122</v>
+        <v>0.844258451508621</v>
       </c>
     </row>
     <row r="8">
@@ -3619,31 +3619,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.996642260759863</v>
+        <v>0.996904353072825</v>
       </c>
       <c r="C8" t="n">
-        <v>0.994821228519139</v>
+        <v>0.994941588616776</v>
       </c>
       <c r="D8" t="n">
-        <v>0.967510194691389</v>
+        <v>0.987159279821831</v>
       </c>
       <c r="E8" t="n">
-        <v>0.980500874128801</v>
+        <v>0.989473391335375</v>
       </c>
       <c r="F8" t="n">
-        <v>0.996642260759863</v>
+        <v>0.996904353072825</v>
       </c>
       <c r="G8" t="n">
-        <v>0.949348722284016</v>
+        <v>0.956710660935478</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.806750270700136</v>
+        <v>0.866678809676326</v>
       </c>
       <c r="J8" t="n">
-        <v>0.862860393593884</v>
+        <v>0.897559879566524</v>
       </c>
     </row>
     <row r="9">
@@ -3651,31 +3651,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.818375625288924</v>
+        <v>0.876244855766799</v>
       </c>
       <c r="C9" t="n">
-        <v>0.820224846236063</v>
+        <v>0.885407614209791</v>
       </c>
       <c r="D9" t="n">
-        <v>0.846858464097846</v>
+        <v>0.860687389076927</v>
       </c>
       <c r="E9" t="n">
-        <v>0.802651934729086</v>
+        <v>0.838878843379912</v>
       </c>
       <c r="F9" t="n">
-        <v>0.818375625288924</v>
+        <v>0.876244855766799</v>
       </c>
       <c r="G9" t="n">
-        <v>0.775872758155764</v>
+        <v>0.813843976608873</v>
       </c>
       <c r="H9" t="n">
-        <v>0.806750270700136</v>
+        <v>0.866678809676326</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.987402673451495</v>
+        <v>0.993877748791142</v>
       </c>
     </row>
     <row r="10">
@@ -3683,28 +3683,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.870977583088279</v>
+        <v>0.904892167412491</v>
       </c>
       <c r="C10" t="n">
-        <v>0.87393226914879</v>
+        <v>0.912659364609705</v>
       </c>
       <c r="D10" t="n">
-        <v>0.886670169863167</v>
+        <v>0.885685258450788</v>
       </c>
       <c r="E10" t="n">
-        <v>0.84453909044488</v>
+        <v>0.867518069945954</v>
       </c>
       <c r="F10" t="n">
-        <v>0.870977583088279</v>
+        <v>0.904892167412491</v>
       </c>
       <c r="G10" t="n">
-        <v>0.823159918238122</v>
+        <v>0.844258451508621</v>
       </c>
       <c r="H10" t="n">
-        <v>0.862860393593884</v>
+        <v>0.897559879566524</v>
       </c>
       <c r="I10" t="n">
-        <v>0.987402673451495</v>
+        <v>0.993877748791142</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -3764,28 +3764,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.556396302897272</v>
+        <v>0.629931704814386</v>
       </c>
       <c r="D2" t="n">
-        <v>0.977810457931385</v>
+        <v>0.963495348698415</v>
       </c>
       <c r="E2" t="n">
-        <v>0.907107075534149</v>
+        <v>0.930087872532394</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.771228859196581</v>
+        <v>0.775488629256279</v>
       </c>
       <c r="H2" t="n">
-        <v>0.849619959923938</v>
+        <v>0.862494112636977</v>
       </c>
       <c r="I2" t="n">
-        <v>0.539095773677176</v>
+        <v>0.595919818033344</v>
       </c>
       <c r="J2" t="n">
-        <v>0.577688204057611</v>
+        <v>0.633050801775934</v>
       </c>
     </row>
     <row r="3">
@@ -3793,31 +3793,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.556396302897272</v>
+        <v>0.629931704814386</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.585018972047965</v>
+        <v>0.574090030056373</v>
       </c>
       <c r="E3" t="n">
-        <v>0.489497093117048</v>
+        <v>0.607560165876334</v>
       </c>
       <c r="F3" t="n">
-        <v>0.556396302897272</v>
+        <v>0.629931704814386</v>
       </c>
       <c r="G3" t="n">
-        <v>0.736565893884078</v>
+        <v>0.75808788658491</v>
       </c>
       <c r="H3" t="n">
-        <v>0.581336746128742</v>
+        <v>0.641976929252869</v>
       </c>
       <c r="I3" t="n">
-        <v>0.638686092201453</v>
+        <v>0.685540312747129</v>
       </c>
       <c r="J3" t="n">
-        <v>0.644652941770622</v>
+        <v>0.693986113716077</v>
       </c>
     </row>
     <row r="4">
@@ -3825,31 +3825,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.977810457931385</v>
+        <v>0.963495348698415</v>
       </c>
       <c r="C4" t="n">
-        <v>0.585018972047965</v>
+        <v>0.574090030056373</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.885609088194205</v>
+        <v>0.960517796812809</v>
       </c>
       <c r="F4" t="n">
-        <v>0.977810457931385</v>
+        <v>0.963495348698415</v>
       </c>
       <c r="G4" t="n">
-        <v>0.78329695678127</v>
+        <v>0.717002061308066</v>
       </c>
       <c r="H4" t="n">
-        <v>0.851307688668939</v>
+        <v>0.842063479944343</v>
       </c>
       <c r="I4" t="n">
-        <v>0.535807864445703</v>
+        <v>0.496185434000178</v>
       </c>
       <c r="J4" t="n">
-        <v>0.569589401443318</v>
+        <v>0.524721005456116</v>
       </c>
     </row>
     <row r="5">
@@ -3857,31 +3857,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.907107075534149</v>
+        <v>0.930087872532394</v>
       </c>
       <c r="C5" t="n">
-        <v>0.489497093117048</v>
+        <v>0.607560165876334</v>
       </c>
       <c r="D5" t="n">
-        <v>0.885609088194205</v>
+        <v>0.960517796812809</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.907107075534149</v>
+        <v>0.930087872532394</v>
       </c>
       <c r="G5" t="n">
-        <v>0.617897912974906</v>
+        <v>0.65515658016706</v>
       </c>
       <c r="H5" t="n">
-        <v>0.786115394996504</v>
+        <v>0.81987321684676</v>
       </c>
       <c r="I5" t="n">
-        <v>0.338156361074165</v>
+        <v>0.402853895519119</v>
       </c>
       <c r="J5" t="n">
-        <v>0.359045449214212</v>
+        <v>0.431096248190475</v>
       </c>
     </row>
     <row r="6">
@@ -3892,28 +3892,28 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.556396302897272</v>
+        <v>0.629931704814386</v>
       </c>
       <c r="D6" t="n">
-        <v>0.977810457931385</v>
+        <v>0.963495348698415</v>
       </c>
       <c r="E6" t="n">
-        <v>0.907107075534149</v>
+        <v>0.930087872532394</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.771228859196581</v>
+        <v>0.775488629256279</v>
       </c>
       <c r="H6" t="n">
-        <v>0.849619959923938</v>
+        <v>0.862494112636977</v>
       </c>
       <c r="I6" t="n">
-        <v>0.539095773677176</v>
+        <v>0.595919818033344</v>
       </c>
       <c r="J6" t="n">
-        <v>0.577688204057611</v>
+        <v>0.633050801775934</v>
       </c>
     </row>
     <row r="7">
@@ -3921,31 +3921,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.771228859196581</v>
+        <v>0.775488629256279</v>
       </c>
       <c r="C7" t="n">
-        <v>0.736565893884078</v>
+        <v>0.75808788658491</v>
       </c>
       <c r="D7" t="n">
-        <v>0.78329695678127</v>
+        <v>0.717002061308066</v>
       </c>
       <c r="E7" t="n">
-        <v>0.617897912974906</v>
+        <v>0.65515658016706</v>
       </c>
       <c r="F7" t="n">
-        <v>0.771228859196581</v>
+        <v>0.775488629256279</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.680809107953649</v>
+        <v>0.698074856262904</v>
       </c>
       <c r="I7" t="n">
-        <v>0.673410805918838</v>
+        <v>0.705721519707372</v>
       </c>
       <c r="J7" t="n">
-        <v>0.68873584366642</v>
+        <v>0.719250971226032</v>
       </c>
     </row>
     <row r="8">
@@ -3953,31 +3953,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.849619959923938</v>
+        <v>0.862494112636977</v>
       </c>
       <c r="C8" t="n">
-        <v>0.581336746128742</v>
+        <v>0.641976929252869</v>
       </c>
       <c r="D8" t="n">
-        <v>0.851307688668939</v>
+        <v>0.842063479944343</v>
       </c>
       <c r="E8" t="n">
-        <v>0.786115394996504</v>
+        <v>0.81987321684676</v>
       </c>
       <c r="F8" t="n">
-        <v>0.849619959923938</v>
+        <v>0.862494112636977</v>
       </c>
       <c r="G8" t="n">
-        <v>0.680809107953649</v>
+        <v>0.698074856262904</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.515526684549171</v>
+        <v>0.563856234957127</v>
       </c>
       <c r="J8" t="n">
-        <v>0.539074657433011</v>
+        <v>0.588421294322135</v>
       </c>
     </row>
     <row r="9">
@@ -3985,31 +3985,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.539095773677176</v>
+        <v>0.595919818033344</v>
       </c>
       <c r="C9" t="n">
-        <v>0.638686092201453</v>
+        <v>0.685540312747129</v>
       </c>
       <c r="D9" t="n">
-        <v>0.535807864445703</v>
+        <v>0.496185434000178</v>
       </c>
       <c r="E9" t="n">
-        <v>0.338156361074165</v>
+        <v>0.402853895519119</v>
       </c>
       <c r="F9" t="n">
-        <v>0.539095773677176</v>
+        <v>0.595919818033344</v>
       </c>
       <c r="G9" t="n">
-        <v>0.673410805918838</v>
+        <v>0.705721519707372</v>
       </c>
       <c r="H9" t="n">
-        <v>0.515526684549171</v>
+        <v>0.563856234957127</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.995640014713203</v>
+        <v>0.996877876300826</v>
       </c>
     </row>
     <row r="10">
@@ -4017,28 +4017,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.577688204057611</v>
+        <v>0.633050801775934</v>
       </c>
       <c r="C10" t="n">
-        <v>0.644652941770622</v>
+        <v>0.693986113716077</v>
       </c>
       <c r="D10" t="n">
-        <v>0.569589401443318</v>
+        <v>0.524721005456116</v>
       </c>
       <c r="E10" t="n">
-        <v>0.359045449214212</v>
+        <v>0.431096248190475</v>
       </c>
       <c r="F10" t="n">
-        <v>0.577688204057611</v>
+        <v>0.633050801775934</v>
       </c>
       <c r="G10" t="n">
-        <v>0.68873584366642</v>
+        <v>0.719250971226032</v>
       </c>
       <c r="H10" t="n">
-        <v>0.539074657433011</v>
+        <v>0.588421294322135</v>
       </c>
       <c r="I10" t="n">
-        <v>0.995640014713203</v>
+        <v>0.996877876300826</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -4098,10 +4098,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.96265405326443</v>
+        <v>0.962654053264432</v>
       </c>
       <c r="D2" t="n">
-        <v>0.915535799339387</v>
+        <v>0.915535799339389</v>
       </c>
       <c r="E2" t="n">
         <v>0.988708912525464</v>
@@ -4110,16 +4110,16 @@
         <v>0.999980538228871</v>
       </c>
       <c r="G2" t="n">
-        <v>0.767439511004778</v>
+        <v>0.767439511004777</v>
       </c>
       <c r="H2" t="n">
-        <v>0.989746461542665</v>
+        <v>0.989746461542666</v>
       </c>
       <c r="I2" t="n">
-        <v>0.658771630910782</v>
+        <v>0.658771630910781</v>
       </c>
       <c r="J2" t="n">
-        <v>0.700252618915961</v>
+        <v>0.697887071680716</v>
       </c>
     </row>
     <row r="3">
@@ -4127,7 +4127,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.96265405326443</v>
+        <v>0.962654053264432</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -4142,7 +4142,7 @@
         <v>0.961936199504099</v>
       </c>
       <c r="G3" t="n">
-        <v>0.727137870197369</v>
+        <v>0.727137870197368</v>
       </c>
       <c r="H3" t="n">
         <v>0.9559542517432</v>
@@ -4151,7 +4151,7 @@
         <v>0.627274806702138</v>
       </c>
       <c r="J3" t="n">
-        <v>0.65689866209369</v>
+        <v>0.656057140776965</v>
       </c>
     </row>
     <row r="4">
@@ -4159,7 +4159,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.915535799339387</v>
+        <v>0.915535799339389</v>
       </c>
       <c r="C4" t="n">
         <v>0.920999442487342</v>
@@ -4174,16 +4174,16 @@
         <v>0.915807005774301</v>
       </c>
       <c r="G4" t="n">
-        <v>0.622266878856807</v>
+        <v>0.622266878856805</v>
       </c>
       <c r="H4" t="n">
-        <v>0.916626661260972</v>
+        <v>0.916626661260973</v>
       </c>
       <c r="I4" t="n">
         <v>0.580978526474961</v>
       </c>
       <c r="J4" t="n">
-        <v>0.583215369183997</v>
+        <v>0.583707398012184</v>
       </c>
     </row>
     <row r="5">
@@ -4206,7 +4206,7 @@
         <v>0.98824180591261</v>
       </c>
       <c r="G5" t="n">
-        <v>0.715281369556585</v>
+        <v>0.715281369556584</v>
       </c>
       <c r="H5" t="n">
         <v>0.974362091499165</v>
@@ -4215,7 +4215,7 @@
         <v>0.645016694048438</v>
       </c>
       <c r="J5" t="n">
-        <v>0.675624053646591</v>
+        <v>0.674814474662788</v>
       </c>
     </row>
     <row r="6">
@@ -4238,16 +4238,16 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.768900746741786</v>
+        <v>0.768900746741785</v>
       </c>
       <c r="H6" t="n">
         <v>0.989828831583144</v>
       </c>
       <c r="I6" t="n">
-        <v>0.657705904477467</v>
+        <v>0.657705904477472</v>
       </c>
       <c r="J6" t="n">
-        <v>0.699357741458237</v>
+        <v>0.696930007694413</v>
       </c>
     </row>
     <row r="7">
@@ -4255,31 +4255,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.767439511004778</v>
+        <v>0.767439511004777</v>
       </c>
       <c r="C7" t="n">
-        <v>0.727137870197369</v>
+        <v>0.727137870197368</v>
       </c>
       <c r="D7" t="n">
-        <v>0.622266878856807</v>
+        <v>0.622266878856805</v>
       </c>
       <c r="E7" t="n">
-        <v>0.715281369556585</v>
+        <v>0.715281369556584</v>
       </c>
       <c r="F7" t="n">
-        <v>0.768900746741786</v>
+        <v>0.768900746741785</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.750908817931184</v>
+        <v>0.750908817931181</v>
       </c>
       <c r="I7" t="n">
-        <v>0.450407365586823</v>
+        <v>0.450407365586822</v>
       </c>
       <c r="J7" t="n">
-        <v>0.490673360621745</v>
+        <v>0.488303657392075</v>
       </c>
     </row>
     <row r="8">
@@ -4287,13 +4287,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.989746461542665</v>
+        <v>0.989746461542666</v>
       </c>
       <c r="C8" t="n">
         <v>0.9559542517432</v>
       </c>
       <c r="D8" t="n">
-        <v>0.916626661260972</v>
+        <v>0.916626661260973</v>
       </c>
       <c r="E8" t="n">
         <v>0.974362091499165</v>
@@ -4302,16 +4302,16 @@
         <v>0.989828831583144</v>
       </c>
       <c r="G8" t="n">
-        <v>0.750908817931184</v>
+        <v>0.750908817931181</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.689231497691716</v>
+        <v>0.689231497691714</v>
       </c>
       <c r="J8" t="n">
-        <v>0.726324587056253</v>
+        <v>0.724165106771902</v>
       </c>
     </row>
     <row r="9">
@@ -4319,7 +4319,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.658771630910782</v>
+        <v>0.658771630910781</v>
       </c>
       <c r="C9" t="n">
         <v>0.627274806702138</v>
@@ -4331,19 +4331,19 @@
         <v>0.645016694048438</v>
       </c>
       <c r="F9" t="n">
-        <v>0.657705904477467</v>
+        <v>0.657705904477472</v>
       </c>
       <c r="G9" t="n">
-        <v>0.450407365586823</v>
+        <v>0.450407365586822</v>
       </c>
       <c r="H9" t="n">
-        <v>0.689231497691716</v>
+        <v>0.689231497691714</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.985378338892117</v>
+        <v>0.988879160438743</v>
       </c>
     </row>
     <row r="10">
@@ -4351,28 +4351,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.700252618915961</v>
+        <v>0.697887071680716</v>
       </c>
       <c r="C10" t="n">
-        <v>0.65689866209369</v>
+        <v>0.656057140776965</v>
       </c>
       <c r="D10" t="n">
-        <v>0.583215369183997</v>
+        <v>0.583707398012184</v>
       </c>
       <c r="E10" t="n">
-        <v>0.675624053646591</v>
+        <v>0.674814474662788</v>
       </c>
       <c r="F10" t="n">
-        <v>0.699357741458237</v>
+        <v>0.696930007694413</v>
       </c>
       <c r="G10" t="n">
-        <v>0.490673360621745</v>
+        <v>0.488303657392075</v>
       </c>
       <c r="H10" t="n">
-        <v>0.726324587056253</v>
+        <v>0.724165106771902</v>
       </c>
       <c r="I10" t="n">
-        <v>0.985378338892117</v>
+        <v>0.988879160438743</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>

</xml_diff>